<commit_message>
fix: add 10% buffer for planning
</commit_message>
<xml_diff>
--- a/app/data/static/samples/by_department/ricotta/2023-09-23 Расписание рикотта.xlsx
+++ b/app/data/static/samples/by_department/ricotta/2023-09-23 Расписание рикотта.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenijkadaner/FileApps/coding_projects/umalat/app/data/static/samples/by_department/ricotta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765F0CEC-72FC-6C44-AFC4-4B6517732AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A7748A-FC6D-764F-9E56-278B931FF2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1553,7 +1553,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4709,9 +4709,9 @@
       <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:160">
+    <row r="1" spans="1:160" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -5190,22 +5190,22 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:160">
+    <row r="2" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:160">
+    <row r="3" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:160">
+    <row r="4" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:160">
+    <row r="5" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:160">
+    <row r="6" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>160</v>
       </c>
@@ -6169,7 +6169,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="7" spans="1:160">
+    <row r="7" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>320</v>
       </c>
@@ -6651,7 +6651,7 @@
         <v>-119</v>
       </c>
     </row>
-    <row r="8" spans="1:160">
+    <row r="8" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>321</v>
       </c>
@@ -7133,7 +7133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:160">
+    <row r="9" spans="1:160" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>322</v>
       </c>
@@ -7634,7 +7634,7 @@
       <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" style="28" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" style="28" customWidth="1"/>
@@ -7648,7 +7648,7 @@
     <col min="18" max="23" width="9.1640625" style="28" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="30" customHeight="1">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>323</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="14" customHeight="1">
+    <row r="2" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>336</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
         <v>340</v>
       </c>
@@ -7784,7 +7784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="40"/>
       <c r="B6" s="40"/>
       <c r="C6" s="20" t="s">
@@ -7809,7 +7809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="40"/>
       <c r="B7" s="40"/>
       <c r="C7" s="20" t="s">
@@ -7834,7 +7834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="40"/>
       <c r="B8" s="40"/>
       <c r="C8" s="20" t="s">
@@ -7859,7 +7859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="39"/>
       <c r="B9" s="39"/>
       <c r="C9" s="20" t="s">
@@ -7884,7 +7884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="s">
         <v>340</v>
       </c>
@@ -7928,7 +7928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="39"/>
       <c r="B13" s="39"/>
       <c r="C13" s="20" t="s">
@@ -7953,7 +7953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="38" t="s">
         <v>349</v>
       </c>
@@ -7997,7 +7997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="39"/>
       <c r="B17" s="39"/>
       <c r="C17" s="20" t="s">
@@ -8022,7 +8022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>353</v>
       </c>
@@ -8066,7 +8066,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="39"/>
       <c r="B21" s="39"/>
       <c r="C21" s="20" t="s">
@@ -8091,7 +8091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="38" t="s">
         <v>355</v>
       </c>
@@ -8135,7 +8135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="39"/>
       <c r="B25" s="39"/>
       <c r="C25" s="20" t="s">
@@ -8160,7 +8160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="38" t="s">
         <v>357</v>
       </c>
@@ -8204,7 +8204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="38" t="s">
         <v>357</v>
       </c>
@@ -8248,7 +8248,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="38" t="s">
         <v>357</v>
       </c>
@@ -8292,7 +8292,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="38" t="s">
         <v>336</v>
       </c>
@@ -8336,7 +8336,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="38" t="s">
         <v>357</v>
       </c>
@@ -8420,10 +8420,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" style="28" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="28" customWidth="1"/>
@@ -8445,7 +8445,7 @@
     <col min="1016" max="1024" width="9.1640625" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="34.25" customHeight="1">
+    <row r="1" spans="1:21" ht="34.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
         <v>364</v>
       </c>
@@ -8491,7 +8491,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="29" customHeight="1">
+    <row r="2" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="46"/>
       <c r="B2" s="46"/>
       <c r="C2" s="46"/>
@@ -8525,7 +8525,7 @@
         <v>2511</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="14" customHeight="1">
+    <row r="3" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24">
         <v>1</v>
       </c>
@@ -8558,7 +8558,7 @@
       </c>
       <c r="R3" s="19"/>
     </row>
-    <row r="4" spans="1:21" ht="14" customHeight="1">
+    <row r="4" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
         <v>379</v>
       </c>
@@ -8598,7 +8598,7 @@
       </c>
       <c r="R4" s="19"/>
     </row>
-    <row r="5" spans="1:21" ht="14" customHeight="1">
+    <row r="5" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24">
         <v>2</v>
       </c>
@@ -8630,7 +8630,7 @@
       </c>
       <c r="R5" s="19"/>
     </row>
-    <row r="6" spans="1:21" ht="14" customHeight="1">
+    <row r="6" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24">
         <v>2</v>
       </c>
@@ -8662,7 +8662,7 @@
       </c>
       <c r="R6" s="19"/>
     </row>
-    <row r="7" spans="1:21" ht="14" customHeight="1">
+    <row r="7" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="24">
         <v>2</v>
       </c>
@@ -8694,7 +8694,7 @@
       </c>
       <c r="R7" s="19"/>
     </row>
-    <row r="8" spans="1:21" ht="9.75" customHeight="1">
+    <row r="8" spans="1:21" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="16" t="s">
         <v>379</v>
       </c>
@@ -8734,7 +8734,7 @@
       </c>
       <c r="R8" s="19"/>
     </row>
-    <row r="9" spans="1:21" ht="14" customHeight="1">
+    <row r="9" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24">
         <v>3</v>
       </c>
@@ -8766,7 +8766,7 @@
       </c>
       <c r="R9" s="19"/>
     </row>
-    <row r="10" spans="1:21" ht="9.75" customHeight="1">
+    <row r="10" spans="1:21" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="16" t="s">
         <v>379</v>
       </c>
@@ -8786,10 +8786,10 @@
         <v>1000</v>
       </c>
       <c r="I10" s="18">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="J10" s="26">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K10" s="25" t="s">
         <v>379</v>
@@ -8806,7 +8806,7 @@
       </c>
       <c r="R10" s="19"/>
     </row>
-    <row r="11" spans="1:21" s="35" customFormat="1" ht="14" customHeight="1">
+    <row r="11" spans="1:21" s="35" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="24">
         <v>3</v>
       </c>
@@ -8838,7 +8838,7 @@
       </c>
       <c r="R11" s="19"/>
     </row>
-    <row r="12" spans="1:21" s="35" customFormat="1" ht="9.75" customHeight="1">
+    <row r="12" spans="1:21" s="35" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="16" t="s">
         <v>379</v>
       </c>
@@ -8879,7 +8879,7 @@
       </c>
       <c r="R12" s="19"/>
     </row>
-    <row r="13" spans="1:21" ht="14" customHeight="1">
+    <row r="13" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="24">
         <v>13</v>
       </c>
@@ -8912,7 +8912,7 @@
       </c>
       <c r="R13" s="19"/>
     </row>
-    <row r="14" spans="1:21" ht="14" customHeight="1">
+    <row r="14" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="16" t="s">
         <v>379</v>
       </c>
@@ -8952,7 +8952,7 @@
       </c>
       <c r="R14" s="19"/>
     </row>
-    <row r="15" spans="1:21" ht="14" customHeight="1">
+    <row r="15" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
       <c r="F15" s="17"/>
@@ -8972,7 +8972,7 @@
       </c>
       <c r="R15" s="19"/>
     </row>
-    <row r="16" spans="1:21" ht="14" customHeight="1">
+    <row r="16" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
       <c r="F16" s="17"/>
@@ -8992,7 +8992,7 @@
       </c>
       <c r="R16" s="19"/>
     </row>
-    <row r="17" spans="2:18" ht="14" customHeight="1">
+    <row r="17" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
       <c r="F17" s="17"/>
@@ -9012,7 +9012,7 @@
       </c>
       <c r="R17" s="19"/>
     </row>
-    <row r="18" spans="2:18" ht="14" customHeight="1">
+    <row r="18" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
       <c r="F18" s="17"/>
@@ -9032,7 +9032,7 @@
       </c>
       <c r="R18" s="19"/>
     </row>
-    <row r="19" spans="2:18" ht="14" customHeight="1">
+    <row r="19" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
       <c r="F19" s="17"/>
@@ -9052,7 +9052,7 @@
       </c>
       <c r="R19" s="19"/>
     </row>
-    <row r="20" spans="2:18" ht="14" customHeight="1">
+    <row r="20" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
       <c r="F20" s="17"/>
@@ -9072,7 +9072,7 @@
       </c>
       <c r="R20" s="19"/>
     </row>
-    <row r="21" spans="2:18" ht="14" customHeight="1">
+    <row r="21" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="F21" s="17"/>
@@ -9092,7 +9092,7 @@
       </c>
       <c r="R21" s="19"/>
     </row>
-    <row r="22" spans="2:18" ht="14" customHeight="1">
+    <row r="22" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="F22" s="17"/>
@@ -9112,7 +9112,7 @@
       </c>
       <c r="R22" s="19"/>
     </row>
-    <row r="23" spans="2:18" ht="14" customHeight="1">
+    <row r="23" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="F23" s="17"/>
@@ -9132,7 +9132,7 @@
       </c>
       <c r="R23" s="19"/>
     </row>
-    <row r="24" spans="2:18" ht="14" customHeight="1">
+    <row r="24" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="F24" s="17"/>
@@ -9152,7 +9152,7 @@
       </c>
       <c r="R24" s="19"/>
     </row>
-    <row r="25" spans="2:18" ht="14" customHeight="1">
+    <row r="25" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="F25" s="17"/>
@@ -9172,7 +9172,7 @@
       </c>
       <c r="R25" s="19"/>
     </row>
-    <row r="26" spans="2:18" ht="14" customHeight="1">
+    <row r="26" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="F26" s="17"/>
@@ -9192,7 +9192,7 @@
       </c>
       <c r="R26" s="19"/>
     </row>
-    <row r="27" spans="2:18" ht="14" customHeight="1">
+    <row r="27" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
       <c r="F27" s="17"/>
@@ -9212,7 +9212,7 @@
       </c>
       <c r="R27" s="19"/>
     </row>
-    <row r="28" spans="2:18" ht="14" customHeight="1">
+    <row r="28" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
       <c r="F28" s="17"/>
@@ -9232,7 +9232,7 @@
       </c>
       <c r="R28" s="19"/>
     </row>
-    <row r="29" spans="2:18" ht="14" customHeight="1">
+    <row r="29" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
       <c r="F29" s="17"/>
@@ -9252,7 +9252,7 @@
       </c>
       <c r="R29" s="19"/>
     </row>
-    <row r="30" spans="2:18" ht="14" customHeight="1">
+    <row r="30" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
       <c r="F30" s="17"/>
@@ -9272,7 +9272,7 @@
       </c>
       <c r="R30" s="19"/>
     </row>
-    <row r="31" spans="2:18" ht="14" customHeight="1">
+    <row r="31" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
       <c r="F31" s="17"/>
@@ -9292,7 +9292,7 @@
       </c>
       <c r="R31" s="19"/>
     </row>
-    <row r="32" spans="2:18" ht="14" customHeight="1">
+    <row r="32" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
       <c r="F32" s="17"/>
@@ -9312,7 +9312,7 @@
       </c>
       <c r="R32" s="19"/>
     </row>
-    <row r="33" spans="2:18" ht="14" customHeight="1">
+    <row r="33" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
       <c r="F33" s="17"/>
@@ -9332,7 +9332,7 @@
       </c>
       <c r="R33" s="19"/>
     </row>
-    <row r="34" spans="2:18" ht="14" customHeight="1">
+    <row r="34" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
       <c r="F34" s="17"/>
@@ -9352,7 +9352,7 @@
       </c>
       <c r="R34" s="19"/>
     </row>
-    <row r="35" spans="2:18" ht="14" customHeight="1">
+    <row r="35" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
       <c r="F35" s="17"/>
@@ -9372,7 +9372,7 @@
       </c>
       <c r="R35" s="19"/>
     </row>
-    <row r="36" spans="2:18" ht="14" customHeight="1">
+    <row r="36" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
       <c r="F36" s="17"/>
@@ -9392,7 +9392,7 @@
       </c>
       <c r="R36" s="19"/>
     </row>
-    <row r="37" spans="2:18" ht="14" customHeight="1">
+    <row r="37" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
       <c r="F37" s="17"/>
@@ -9412,7 +9412,7 @@
       </c>
       <c r="R37" s="19"/>
     </row>
-    <row r="38" spans="2:18" ht="14" customHeight="1">
+    <row r="38" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
       <c r="F38" s="17"/>
@@ -9432,7 +9432,7 @@
       </c>
       <c r="R38" s="19"/>
     </row>
-    <row r="39" spans="2:18" ht="14" customHeight="1">
+    <row r="39" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
       <c r="F39" s="17"/>
@@ -9452,7 +9452,7 @@
       </c>
       <c r="R39" s="19"/>
     </row>
-    <row r="40" spans="2:18" ht="14" customHeight="1">
+    <row r="40" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
       <c r="F40" s="17"/>
@@ -9472,7 +9472,7 @@
       </c>
       <c r="R40" s="19"/>
     </row>
-    <row r="41" spans="2:18" ht="14" customHeight="1">
+    <row r="41" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
       <c r="F41" s="17"/>
@@ -9492,7 +9492,7 @@
       </c>
       <c r="R41" s="19"/>
     </row>
-    <row r="42" spans="2:18" ht="14" customHeight="1">
+    <row r="42" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
       <c r="F42" s="17"/>
@@ -9512,7 +9512,7 @@
       </c>
       <c r="R42" s="19"/>
     </row>
-    <row r="43" spans="2:18" ht="14" customHeight="1">
+    <row r="43" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
       <c r="F43" s="17"/>
@@ -9532,7 +9532,7 @@
       </c>
       <c r="R43" s="19"/>
     </row>
-    <row r="44" spans="2:18" ht="14" customHeight="1">
+    <row r="44" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
       <c r="F44" s="17"/>
@@ -9552,7 +9552,7 @@
       </c>
       <c r="R44" s="19"/>
     </row>
-    <row r="45" spans="2:18" ht="14" customHeight="1">
+    <row r="45" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
       <c r="F45" s="17"/>
@@ -9572,7 +9572,7 @@
       </c>
       <c r="R45" s="19"/>
     </row>
-    <row r="46" spans="2:18" ht="14" customHeight="1">
+    <row r="46" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
       <c r="F46" s="17"/>
@@ -9592,7 +9592,7 @@
       </c>
       <c r="R46" s="19"/>
     </row>
-    <row r="47" spans="2:18" ht="14" customHeight="1">
+    <row r="47" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
       <c r="F47" s="17"/>
@@ -9612,7 +9612,7 @@
       </c>
       <c r="R47" s="19"/>
     </row>
-    <row r="48" spans="2:18" ht="14" customHeight="1">
+    <row r="48" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="16"/>
       <c r="C48" s="16"/>
       <c r="F48" s="17"/>
@@ -9632,7 +9632,7 @@
       </c>
       <c r="R48" s="19"/>
     </row>
-    <row r="49" spans="2:18" ht="14" customHeight="1">
+    <row r="49" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="16"/>
       <c r="C49" s="16"/>
       <c r="F49" s="17"/>
@@ -9652,7 +9652,7 @@
       </c>
       <c r="R49" s="19"/>
     </row>
-    <row r="50" spans="2:18" ht="14" customHeight="1">
+    <row r="50" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="16"/>
       <c r="C50" s="16"/>
       <c r="F50" s="17"/>
@@ -9672,7 +9672,7 @@
       </c>
       <c r="R50" s="19"/>
     </row>
-    <row r="51" spans="2:18" ht="14" customHeight="1">
+    <row r="51" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="16"/>
       <c r="C51" s="16"/>
       <c r="F51" s="17"/>
@@ -9692,7 +9692,7 @@
       </c>
       <c r="R51" s="19"/>
     </row>
-    <row r="52" spans="2:18" ht="14" customHeight="1">
+    <row r="52" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="16"/>
       <c r="C52" s="16"/>
       <c r="F52" s="17"/>
@@ -9712,7 +9712,7 @@
       </c>
       <c r="R52" s="19"/>
     </row>
-    <row r="53" spans="2:18" ht="14" customHeight="1">
+    <row r="53" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="16"/>
       <c r="C53" s="16"/>
       <c r="F53" s="17"/>
@@ -9732,7 +9732,7 @@
       </c>
       <c r="R53" s="19"/>
     </row>
-    <row r="54" spans="2:18" ht="14" customHeight="1">
+    <row r="54" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="16"/>
       <c r="C54" s="16"/>
       <c r="F54" s="17"/>
@@ -9752,7 +9752,7 @@
       </c>
       <c r="R54" s="19"/>
     </row>
-    <row r="55" spans="2:18" ht="14" customHeight="1">
+    <row r="55" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="16"/>
       <c r="C55" s="16"/>
       <c r="F55" s="17"/>
@@ -9772,7 +9772,7 @@
       </c>
       <c r="R55" s="19"/>
     </row>
-    <row r="56" spans="2:18" ht="14" customHeight="1">
+    <row r="56" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
       <c r="F56" s="17"/>
@@ -9792,7 +9792,7 @@
       </c>
       <c r="R56" s="19"/>
     </row>
-    <row r="57" spans="2:18" ht="14" customHeight="1">
+    <row r="57" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="16"/>
       <c r="C57" s="16"/>
       <c r="F57" s="17"/>
@@ -9812,7 +9812,7 @@
       </c>
       <c r="R57" s="19"/>
     </row>
-    <row r="58" spans="2:18" ht="14" customHeight="1">
+    <row r="58" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="16"/>
       <c r="C58" s="16"/>
       <c r="F58" s="17"/>
@@ -9832,7 +9832,7 @@
       </c>
       <c r="R58" s="19"/>
     </row>
-    <row r="59" spans="2:18" ht="14" customHeight="1">
+    <row r="59" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="16"/>
       <c r="C59" s="16"/>
       <c r="F59" s="17"/>
@@ -9852,7 +9852,7 @@
       </c>
       <c r="R59" s="19"/>
     </row>
-    <row r="60" spans="2:18" ht="14" customHeight="1">
+    <row r="60" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="16"/>
       <c r="C60" s="16"/>
       <c r="F60" s="17"/>
@@ -9872,7 +9872,7 @@
       </c>
       <c r="R60" s="19"/>
     </row>
-    <row r="61" spans="2:18" ht="14" customHeight="1">
+    <row r="61" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="16"/>
       <c r="C61" s="16"/>
       <c r="F61" s="17"/>
@@ -9892,7 +9892,7 @@
       </c>
       <c r="R61" s="19"/>
     </row>
-    <row r="62" spans="2:18" ht="14" customHeight="1">
+    <row r="62" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="16"/>
       <c r="C62" s="16"/>
       <c r="F62" s="17"/>
@@ -9912,7 +9912,7 @@
       </c>
       <c r="R62" s="19"/>
     </row>
-    <row r="63" spans="2:18" ht="14" customHeight="1">
+    <row r="63" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="16"/>
       <c r="C63" s="16"/>
       <c r="F63" s="17"/>
@@ -9932,7 +9932,7 @@
       </c>
       <c r="R63" s="19"/>
     </row>
-    <row r="64" spans="2:18" ht="14" customHeight="1">
+    <row r="64" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="16"/>
       <c r="C64" s="16"/>
       <c r="F64" s="17"/>
@@ -9952,7 +9952,7 @@
       </c>
       <c r="R64" s="19"/>
     </row>
-    <row r="65" spans="2:18" ht="14" customHeight="1">
+    <row r="65" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="16"/>
       <c r="C65" s="16"/>
       <c r="F65" s="17"/>
@@ -9972,7 +9972,7 @@
       </c>
       <c r="R65" s="19"/>
     </row>
-    <row r="66" spans="2:18" ht="14" customHeight="1">
+    <row r="66" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="16"/>
       <c r="C66" s="16"/>
       <c r="F66" s="17"/>
@@ -9992,7 +9992,7 @@
       </c>
       <c r="R66" s="19"/>
     </row>
-    <row r="67" spans="2:18" ht="14" customHeight="1">
+    <row r="67" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="16"/>
       <c r="C67" s="16"/>
       <c r="F67" s="17"/>
@@ -10012,7 +10012,7 @@
       </c>
       <c r="R67" s="19"/>
     </row>
-    <row r="68" spans="2:18" ht="14" customHeight="1">
+    <row r="68" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="16"/>
       <c r="C68" s="16"/>
       <c r="F68" s="17"/>
@@ -10032,7 +10032,7 @@
       </c>
       <c r="R68" s="19"/>
     </row>
-    <row r="69" spans="2:18" ht="14" customHeight="1">
+    <row r="69" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="16"/>
       <c r="C69" s="16"/>
       <c r="F69" s="17"/>
@@ -10052,7 +10052,7 @@
       </c>
       <c r="R69" s="19"/>
     </row>
-    <row r="70" spans="2:18" ht="14" customHeight="1">
+    <row r="70" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="16"/>
       <c r="C70" s="16"/>
       <c r="F70" s="17"/>
@@ -10072,7 +10072,7 @@
       </c>
       <c r="R70" s="19"/>
     </row>
-    <row r="71" spans="2:18" ht="14" customHeight="1">
+    <row r="71" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="16"/>
       <c r="C71" s="16"/>
       <c r="F71" s="17"/>
@@ -10092,7 +10092,7 @@
       </c>
       <c r="R71" s="19"/>
     </row>
-    <row r="72" spans="2:18" ht="14" customHeight="1">
+    <row r="72" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="16"/>
       <c r="C72" s="16"/>
       <c r="F72" s="17"/>
@@ -10112,7 +10112,7 @@
       </c>
       <c r="R72" s="19"/>
     </row>
-    <row r="73" spans="2:18" ht="14" customHeight="1">
+    <row r="73" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="16"/>
       <c r="C73" s="16"/>
       <c r="F73" s="17"/>
@@ -10132,7 +10132,7 @@
       </c>
       <c r="R73" s="19"/>
     </row>
-    <row r="74" spans="2:18" ht="14" customHeight="1">
+    <row r="74" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="16"/>
       <c r="C74" s="16"/>
       <c r="F74" s="17"/>
@@ -10152,7 +10152,7 @@
       </c>
       <c r="R74" s="19"/>
     </row>
-    <row r="75" spans="2:18" ht="14" customHeight="1">
+    <row r="75" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="16"/>
       <c r="C75" s="16"/>
       <c r="F75" s="17"/>
@@ -10172,7 +10172,7 @@
       </c>
       <c r="R75" s="19"/>
     </row>
-    <row r="76" spans="2:18" ht="14" customHeight="1">
+    <row r="76" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="16"/>
       <c r="C76" s="16"/>
       <c r="F76" s="17"/>
@@ -10192,7 +10192,7 @@
       </c>
       <c r="R76" s="19"/>
     </row>
-    <row r="77" spans="2:18" ht="14" customHeight="1">
+    <row r="77" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="16"/>
       <c r="C77" s="16"/>
       <c r="F77" s="17"/>
@@ -10212,7 +10212,7 @@
       </c>
       <c r="R77" s="19"/>
     </row>
-    <row r="78" spans="2:18" ht="14" customHeight="1">
+    <row r="78" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="16"/>
       <c r="C78" s="16"/>
       <c r="F78" s="17"/>
@@ -10232,7 +10232,7 @@
       </c>
       <c r="R78" s="19"/>
     </row>
-    <row r="79" spans="2:18" ht="14" customHeight="1">
+    <row r="79" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="16"/>
       <c r="C79" s="16"/>
       <c r="F79" s="17"/>
@@ -10252,7 +10252,7 @@
       </c>
       <c r="R79" s="19"/>
     </row>
-    <row r="80" spans="2:18" ht="14" customHeight="1">
+    <row r="80" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="16"/>
       <c r="C80" s="16"/>
       <c r="F80" s="17"/>
@@ -10272,7 +10272,7 @@
       </c>
       <c r="R80" s="19"/>
     </row>
-    <row r="81" spans="2:18" ht="14" customHeight="1">
+    <row r="81" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="16"/>
       <c r="C81" s="16"/>
       <c r="F81" s="17"/>
@@ -10292,7 +10292,7 @@
       </c>
       <c r="R81" s="19"/>
     </row>
-    <row r="82" spans="2:18" ht="14" customHeight="1">
+    <row r="82" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="16"/>
       <c r="C82" s="16"/>
       <c r="F82" s="17"/>
@@ -10312,7 +10312,7 @@
       </c>
       <c r="R82" s="19"/>
     </row>
-    <row r="83" spans="2:18" ht="14" customHeight="1">
+    <row r="83" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="16"/>
       <c r="C83" s="16"/>
       <c r="F83" s="17"/>
@@ -10332,7 +10332,7 @@
       </c>
       <c r="R83" s="19"/>
     </row>
-    <row r="84" spans="2:18" ht="14" customHeight="1">
+    <row r="84" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="16"/>
       <c r="C84" s="16"/>
       <c r="F84" s="17"/>
@@ -10352,7 +10352,7 @@
       </c>
       <c r="R84" s="19"/>
     </row>
-    <row r="85" spans="2:18" ht="14" customHeight="1">
+    <row r="85" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B85" s="16"/>
       <c r="C85" s="16"/>
       <c r="F85" s="17"/>
@@ -10372,7 +10372,7 @@
       </c>
       <c r="R85" s="19"/>
     </row>
-    <row r="86" spans="2:18" ht="14" customHeight="1">
+    <row r="86" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="16"/>
       <c r="C86" s="16"/>
       <c r="F86" s="17"/>
@@ -10392,7 +10392,7 @@
       </c>
       <c r="R86" s="19"/>
     </row>
-    <row r="87" spans="2:18" ht="14" customHeight="1">
+    <row r="87" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="16"/>
       <c r="C87" s="16"/>
       <c r="F87" s="17"/>
@@ -10412,7 +10412,7 @@
       </c>
       <c r="R87" s="19"/>
     </row>
-    <row r="88" spans="2:18" ht="14" customHeight="1">
+    <row r="88" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="16"/>
       <c r="C88" s="16"/>
       <c r="F88" s="17"/>
@@ -10432,7 +10432,7 @@
       </c>
       <c r="R88" s="19"/>
     </row>
-    <row r="89" spans="2:18" ht="14" customHeight="1">
+    <row r="89" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B89" s="16"/>
       <c r="C89" s="16"/>
       <c r="F89" s="17"/>
@@ -10452,7 +10452,7 @@
       </c>
       <c r="R89" s="19"/>
     </row>
-    <row r="90" spans="2:18" ht="14" customHeight="1">
+    <row r="90" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="16"/>
       <c r="C90" s="16"/>
       <c r="F90" s="17"/>
@@ -10472,7 +10472,7 @@
       </c>
       <c r="R90" s="19"/>
     </row>
-    <row r="91" spans="2:18" ht="14" customHeight="1">
+    <row r="91" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="16"/>
       <c r="C91" s="16"/>
       <c r="F91" s="17"/>
@@ -10492,7 +10492,7 @@
       </c>
       <c r="R91" s="19"/>
     </row>
-    <row r="92" spans="2:18" ht="14" customHeight="1">
+    <row r="92" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B92" s="16"/>
       <c r="C92" s="16"/>
       <c r="F92" s="17"/>
@@ -10512,7 +10512,7 @@
       </c>
       <c r="R92" s="19"/>
     </row>
-    <row r="93" spans="2:18" ht="14" customHeight="1">
+    <row r="93" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B93" s="16"/>
       <c r="C93" s="16"/>
       <c r="F93" s="17"/>
@@ -10532,7 +10532,7 @@
       </c>
       <c r="R93" s="19"/>
     </row>
-    <row r="94" spans="2:18" ht="14" customHeight="1">
+    <row r="94" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B94" s="16"/>
       <c r="C94" s="16"/>
       <c r="F94" s="17"/>
@@ -10552,7 +10552,7 @@
       </c>
       <c r="R94" s="19"/>
     </row>
-    <row r="95" spans="2:18" ht="14" customHeight="1">
+    <row r="95" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" s="16"/>
       <c r="C95" s="16"/>
       <c r="F95" s="17"/>
@@ -10572,7 +10572,7 @@
       </c>
       <c r="R95" s="19"/>
     </row>
-    <row r="96" spans="2:18" ht="14" customHeight="1">
+    <row r="96" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B96" s="16"/>
       <c r="C96" s="16"/>
       <c r="F96" s="17"/>
@@ -10592,7 +10592,7 @@
       </c>
       <c r="R96" s="19"/>
     </row>
-    <row r="97" spans="2:18" ht="14" customHeight="1">
+    <row r="97" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="16"/>
       <c r="C97" s="16"/>
       <c r="F97" s="17"/>
@@ -10612,7 +10612,7 @@
       </c>
       <c r="R97" s="19"/>
     </row>
-    <row r="98" spans="2:18" ht="14" customHeight="1">
+    <row r="98" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B98" s="16"/>
       <c r="C98" s="16"/>
       <c r="F98" s="17"/>
@@ -10632,7 +10632,7 @@
       </c>
       <c r="R98" s="19"/>
     </row>
-    <row r="99" spans="2:18" ht="14" customHeight="1">
+    <row r="99" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" s="16"/>
       <c r="C99" s="16"/>
       <c r="F99" s="17"/>
@@ -10652,7 +10652,7 @@
       </c>
       <c r="R99" s="19"/>
     </row>
-    <row r="100" spans="2:18" ht="14" customHeight="1">
+    <row r="100" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="16"/>
       <c r="C100" s="16"/>
       <c r="F100" s="17"/>
@@ -10672,7 +10672,7 @@
       </c>
       <c r="R100" s="19"/>
     </row>
-    <row r="101" spans="2:18" ht="14" customHeight="1">
+    <row r="101" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="16"/>
       <c r="C101" s="16"/>
       <c r="F101" s="17"/>
@@ -10692,7 +10692,7 @@
       </c>
       <c r="R101" s="19"/>
     </row>
-    <row r="102" spans="2:18" ht="14" customHeight="1">
+    <row r="102" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B102" s="16"/>
       <c r="C102" s="16"/>
       <c r="F102" s="17"/>
@@ -10712,7 +10712,7 @@
       </c>
       <c r="R102" s="19"/>
     </row>
-    <row r="103" spans="2:18" ht="14" customHeight="1">
+    <row r="103" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B103" s="16"/>
       <c r="C103" s="16"/>
       <c r="F103" s="17"/>
@@ -10732,7 +10732,7 @@
       </c>
       <c r="R103" s="19"/>
     </row>
-    <row r="104" spans="2:18" ht="14" customHeight="1">
+    <row r="104" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B104" s="16"/>
       <c r="C104" s="16"/>
       <c r="F104" s="17"/>
@@ -10752,7 +10752,7 @@
       </c>
       <c r="R104" s="19"/>
     </row>
-    <row r="105" spans="2:18" ht="14" customHeight="1">
+    <row r="105" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="16"/>
       <c r="C105" s="16"/>
       <c r="F105" s="17"/>
@@ -10772,7 +10772,7 @@
       </c>
       <c r="R105" s="19"/>
     </row>
-    <row r="106" spans="2:18" ht="14" customHeight="1">
+    <row r="106" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B106" s="16"/>
       <c r="C106" s="16"/>
       <c r="F106" s="17"/>
@@ -10792,7 +10792,7 @@
       </c>
       <c r="R106" s="19"/>
     </row>
-    <row r="107" spans="2:18" ht="14" customHeight="1">
+    <row r="107" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B107" s="16"/>
       <c r="C107" s="16"/>
       <c r="F107" s="17"/>
@@ -10812,7 +10812,7 @@
       </c>
       <c r="R107" s="19"/>
     </row>
-    <row r="108" spans="2:18" ht="14" customHeight="1">
+    <row r="108" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B108" s="16"/>
       <c r="C108" s="16"/>
       <c r="F108" s="17"/>
@@ -10832,7 +10832,7 @@
       </c>
       <c r="R108" s="19"/>
     </row>
-    <row r="109" spans="2:18" ht="14" customHeight="1">
+    <row r="109" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="16"/>
       <c r="C109" s="16"/>
       <c r="F109" s="17"/>
@@ -10852,7 +10852,7 @@
       </c>
       <c r="R109" s="19"/>
     </row>
-    <row r="110" spans="2:18" ht="14" customHeight="1">
+    <row r="110" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="16"/>
       <c r="C110" s="16"/>
       <c r="F110" s="17"/>
@@ -10872,7 +10872,7 @@
       </c>
       <c r="R110" s="19"/>
     </row>
-    <row r="111" spans="2:18" ht="14" customHeight="1">
+    <row r="111" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B111" s="16"/>
       <c r="C111" s="16"/>
       <c r="F111" s="17"/>
@@ -10892,7 +10892,7 @@
       </c>
       <c r="R111" s="19"/>
     </row>
-    <row r="112" spans="2:18" ht="14" customHeight="1">
+    <row r="112" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B112" s="16"/>
       <c r="C112" s="16"/>
       <c r="F112" s="17"/>
@@ -10912,7 +10912,7 @@
       </c>
       <c r="R112" s="19"/>
     </row>
-    <row r="113" spans="2:18" ht="14" customHeight="1">
+    <row r="113" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B113" s="16"/>
       <c r="C113" s="16"/>
       <c r="F113" s="17"/>
@@ -10932,7 +10932,7 @@
       </c>
       <c r="R113" s="19"/>
     </row>
-    <row r="114" spans="2:18" ht="14" customHeight="1">
+    <row r="114" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B114" s="16"/>
       <c r="C114" s="16"/>
       <c r="F114" s="17"/>
@@ -10952,7 +10952,7 @@
       </c>
       <c r="R114" s="19"/>
     </row>
-    <row r="115" spans="2:18" ht="14" customHeight="1">
+    <row r="115" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="16"/>
       <c r="C115" s="16"/>
       <c r="F115" s="17"/>
@@ -10972,7 +10972,7 @@
       </c>
       <c r="R115" s="19"/>
     </row>
-    <row r="116" spans="2:18" ht="14" customHeight="1">
+    <row r="116" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B116" s="16"/>
       <c r="C116" s="16"/>
       <c r="F116" s="17"/>
@@ -10982,7 +10982,7 @@
       <c r="J116" s="18"/>
       <c r="R116" s="19"/>
     </row>
-    <row r="117" spans="2:18" ht="14" customHeight="1">
+    <row r="117" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B117" s="16"/>
       <c r="C117" s="16"/>
       <c r="F117" s="17"/>
@@ -10992,7 +10992,7 @@
       <c r="J117" s="18"/>
       <c r="R117" s="19"/>
     </row>
-    <row r="118" spans="2:18" ht="14" customHeight="1">
+    <row r="118" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B118" s="16"/>
       <c r="C118" s="16"/>
       <c r="F118" s="17"/>
@@ -11002,7 +11002,7 @@
       <c r="J118" s="18"/>
       <c r="R118" s="19"/>
     </row>
-    <row r="119" spans="2:18" ht="14" customHeight="1">
+    <row r="119" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="16"/>
       <c r="C119" s="16"/>
       <c r="F119" s="17"/>
@@ -11012,7 +11012,7 @@
       <c r="J119" s="18"/>
       <c r="R119" s="19"/>
     </row>
-    <row r="120" spans="2:18" ht="14" customHeight="1">
+    <row r="120" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B120" s="16"/>
       <c r="C120" s="16"/>
       <c r="F120" s="17"/>
@@ -11022,7 +11022,7 @@
       <c r="J120" s="18"/>
       <c r="R120" s="19"/>
     </row>
-    <row r="121" spans="2:18" ht="14" customHeight="1">
+    <row r="121" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B121" s="16"/>
       <c r="C121" s="16"/>
       <c r="F121" s="17"/>
@@ -11032,7 +11032,7 @@
       <c r="J121" s="18"/>
       <c r="R121" s="19"/>
     </row>
-    <row r="122" spans="2:18" ht="14" customHeight="1">
+    <row r="122" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B122" s="16"/>
       <c r="C122" s="16"/>
       <c r="F122" s="17"/>
@@ -11042,7 +11042,7 @@
       <c r="J122" s="18"/>
       <c r="R122" s="19"/>
     </row>
-    <row r="123" spans="2:18" ht="14" customHeight="1">
+    <row r="123" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B123" s="16"/>
       <c r="C123" s="16"/>
       <c r="F123" s="17"/>
@@ -11052,7 +11052,7 @@
       <c r="J123" s="18"/>
       <c r="R123" s="19"/>
     </row>
-    <row r="124" spans="2:18" ht="14" customHeight="1">
+    <row r="124" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B124" s="16"/>
       <c r="C124" s="16"/>
       <c r="F124" s="17"/>
@@ -11062,7 +11062,7 @@
       <c r="J124" s="18"/>
       <c r="R124" s="19"/>
     </row>
-    <row r="125" spans="2:18" ht="14" customHeight="1">
+    <row r="125" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B125" s="16"/>
       <c r="C125" s="16"/>
       <c r="F125" s="17"/>
@@ -11072,7 +11072,7 @@
       <c r="J125" s="18"/>
       <c r="R125" s="19"/>
     </row>
-    <row r="126" spans="2:18" ht="14" customHeight="1">
+    <row r="126" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B126" s="16"/>
       <c r="C126" s="16"/>
       <c r="F126" s="17"/>
@@ -11082,7 +11082,7 @@
       <c r="J126" s="18"/>
       <c r="R126" s="19"/>
     </row>
-    <row r="127" spans="2:18" ht="14" customHeight="1">
+    <row r="127" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B127" s="16"/>
       <c r="C127" s="16"/>
       <c r="F127" s="17"/>
@@ -11092,7 +11092,7 @@
       <c r="J127" s="18"/>
       <c r="R127" s="19"/>
     </row>
-    <row r="128" spans="2:18" ht="14" customHeight="1">
+    <row r="128" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B128" s="16"/>
       <c r="C128" s="16"/>
       <c r="F128" s="17"/>
@@ -11102,7 +11102,7 @@
       <c r="J128" s="18"/>
       <c r="R128" s="19"/>
     </row>
-    <row r="129" spans="2:18" ht="14" customHeight="1">
+    <row r="129" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B129" s="16"/>
       <c r="C129" s="16"/>
       <c r="F129" s="17"/>
@@ -11112,7 +11112,7 @@
       <c r="J129" s="18"/>
       <c r="R129" s="19"/>
     </row>
-    <row r="130" spans="2:18" ht="14" customHeight="1">
+    <row r="130" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B130" s="16"/>
       <c r="C130" s="16"/>
       <c r="F130" s="17"/>
@@ -11122,7 +11122,7 @@
       <c r="J130" s="18"/>
       <c r="R130" s="19"/>
     </row>
-    <row r="131" spans="2:18" ht="14" customHeight="1">
+    <row r="131" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B131" s="16"/>
       <c r="C131" s="16"/>
       <c r="F131" s="17"/>
@@ -11132,7 +11132,7 @@
       <c r="J131" s="18"/>
       <c r="R131" s="19"/>
     </row>
-    <row r="132" spans="2:18" ht="14" customHeight="1">
+    <row r="132" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B132" s="16"/>
       <c r="C132" s="16"/>
       <c r="F132" s="17"/>
@@ -11142,7 +11142,7 @@
       <c r="J132" s="18"/>
       <c r="R132" s="19"/>
     </row>
-    <row r="133" spans="2:18" ht="14" customHeight="1">
+    <row r="133" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B133" s="16"/>
       <c r="C133" s="16"/>
       <c r="F133" s="17"/>
@@ -11152,7 +11152,7 @@
       <c r="J133" s="18"/>
       <c r="R133" s="19"/>
     </row>
-    <row r="134" spans="2:18" ht="14" customHeight="1">
+    <row r="134" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B134" s="16"/>
       <c r="C134" s="16"/>
       <c r="F134" s="17"/>
@@ -11162,7 +11162,7 @@
       <c r="J134" s="18"/>
       <c r="R134" s="19"/>
     </row>
-    <row r="135" spans="2:18" ht="14" customHeight="1">
+    <row r="135" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B135" s="16"/>
       <c r="C135" s="16"/>
       <c r="F135" s="17"/>
@@ -11172,7 +11172,7 @@
       <c r="J135" s="18"/>
       <c r="R135" s="19"/>
     </row>
-    <row r="136" spans="2:18" ht="14" customHeight="1">
+    <row r="136" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B136" s="16"/>
       <c r="C136" s="16"/>
       <c r="F136" s="17"/>
@@ -11182,7 +11182,7 @@
       <c r="J136" s="18"/>
       <c r="R136" s="19"/>
     </row>
-    <row r="137" spans="2:18" ht="14" customHeight="1">
+    <row r="137" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B137" s="16"/>
       <c r="C137" s="16"/>
       <c r="F137" s="17"/>
@@ -11192,7 +11192,7 @@
       <c r="J137" s="18"/>
       <c r="R137" s="19"/>
     </row>
-    <row r="138" spans="2:18" ht="14" customHeight="1">
+    <row r="138" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B138" s="16"/>
       <c r="C138" s="16"/>
       <c r="F138" s="17"/>
@@ -11202,7 +11202,7 @@
       <c r="J138" s="18"/>
       <c r="R138" s="19"/>
     </row>
-    <row r="139" spans="2:18" ht="14" customHeight="1">
+    <row r="139" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B139" s="16"/>
       <c r="C139" s="16"/>
       <c r="F139" s="17"/>
@@ -11212,7 +11212,7 @@
       <c r="J139" s="18"/>
       <c r="R139" s="19"/>
     </row>
-    <row r="140" spans="2:18" ht="14" customHeight="1">
+    <row r="140" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B140" s="16"/>
       <c r="C140" s="16"/>
       <c r="F140" s="17"/>
@@ -11222,7 +11222,7 @@
       <c r="J140" s="18"/>
       <c r="R140" s="19"/>
     </row>
-    <row r="141" spans="2:18" ht="14" customHeight="1">
+    <row r="141" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B141" s="16"/>
       <c r="C141" s="16"/>
       <c r="F141" s="17"/>
@@ -11232,7 +11232,7 @@
       <c r="J141" s="18"/>
       <c r="R141" s="19"/>
     </row>
-    <row r="142" spans="2:18" ht="14" customHeight="1">
+    <row r="142" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B142" s="16"/>
       <c r="C142" s="16"/>
       <c r="F142" s="17"/>
@@ -11242,7 +11242,7 @@
       <c r="J142" s="18"/>
       <c r="R142" s="19"/>
     </row>
-    <row r="143" spans="2:18" ht="14" customHeight="1">
+    <row r="143" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B143" s="16"/>
       <c r="C143" s="16"/>
       <c r="F143" s="17"/>
@@ -11252,7 +11252,7 @@
       <c r="J143" s="18"/>
       <c r="R143" s="19"/>
     </row>
-    <row r="144" spans="2:18" ht="14" customHeight="1">
+    <row r="144" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B144" s="16"/>
       <c r="C144" s="16"/>
       <c r="F144" s="17"/>
@@ -11262,7 +11262,7 @@
       <c r="J144" s="18"/>
       <c r="R144" s="19"/>
     </row>
-    <row r="145" spans="2:18" ht="14" customHeight="1">
+    <row r="145" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B145" s="16"/>
       <c r="C145" s="16"/>
       <c r="F145" s="17"/>
@@ -11272,7 +11272,7 @@
       <c r="J145" s="18"/>
       <c r="R145" s="19"/>
     </row>
-    <row r="146" spans="2:18" ht="14" customHeight="1">
+    <row r="146" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B146" s="16"/>
       <c r="C146" s="16"/>
       <c r="F146" s="17"/>
@@ -11282,7 +11282,7 @@
       <c r="J146" s="18"/>
       <c r="R146" s="19"/>
     </row>
-    <row r="147" spans="2:18" ht="14" customHeight="1">
+    <row r="147" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B147" s="16"/>
       <c r="C147" s="16"/>
       <c r="F147" s="17"/>
@@ -11292,7 +11292,7 @@
       <c r="J147" s="18"/>
       <c r="R147" s="19"/>
     </row>
-    <row r="148" spans="2:18" ht="14" customHeight="1">
+    <row r="148" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B148" s="16"/>
       <c r="C148" s="16"/>
       <c r="F148" s="17"/>
@@ -11302,7 +11302,7 @@
       <c r="J148" s="18"/>
       <c r="R148" s="19"/>
     </row>
-    <row r="149" spans="2:18" ht="14" customHeight="1">
+    <row r="149" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B149" s="16"/>
       <c r="C149" s="16"/>
       <c r="F149" s="17"/>
@@ -11312,7 +11312,7 @@
       <c r="J149" s="18"/>
       <c r="R149" s="19"/>
     </row>
-    <row r="150" spans="2:18" ht="14" customHeight="1">
+    <row r="150" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B150" s="16"/>
       <c r="C150" s="16"/>
       <c r="F150" s="17"/>
@@ -11322,7 +11322,7 @@
       <c r="J150" s="18"/>
       <c r="R150" s="19"/>
     </row>
-    <row r="151" spans="2:18" ht="14" customHeight="1">
+    <row r="151" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B151" s="16"/>
       <c r="C151" s="16"/>
       <c r="F151" s="17"/>
@@ -11332,7 +11332,7 @@
       <c r="J151" s="18"/>
       <c r="R151" s="19"/>
     </row>
-    <row r="152" spans="2:18" ht="14" customHeight="1">
+    <row r="152" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B152" s="16"/>
       <c r="C152" s="16"/>
       <c r="F152" s="17"/>
@@ -11342,7 +11342,7 @@
       <c r="J152" s="18"/>
       <c r="R152" s="19"/>
     </row>
-    <row r="153" spans="2:18" ht="14" customHeight="1">
+    <row r="153" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B153" s="16"/>
       <c r="C153" s="16"/>
       <c r="F153" s="17"/>
@@ -11352,7 +11352,7 @@
       <c r="J153" s="18"/>
       <c r="R153" s="19"/>
     </row>
-    <row r="154" spans="2:18" ht="14" customHeight="1">
+    <row r="154" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B154" s="16"/>
       <c r="C154" s="16"/>
       <c r="F154" s="17"/>
@@ -11362,7 +11362,7 @@
       <c r="J154" s="18"/>
       <c r="R154" s="19"/>
     </row>
-    <row r="155" spans="2:18" ht="14" customHeight="1">
+    <row r="155" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B155" s="16"/>
       <c r="C155" s="16"/>
       <c r="F155" s="17"/>
@@ -11372,7 +11372,7 @@
       <c r="J155" s="18"/>
       <c r="R155" s="19"/>
     </row>
-    <row r="156" spans="2:18" ht="14" customHeight="1">
+    <row r="156" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B156" s="16"/>
       <c r="C156" s="16"/>
       <c r="F156" s="17"/>
@@ -11382,7 +11382,7 @@
       <c r="J156" s="18"/>
       <c r="R156" s="19"/>
     </row>
-    <row r="157" spans="2:18" ht="14" customHeight="1">
+    <row r="157" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B157" s="16"/>
       <c r="C157" s="16"/>
       <c r="F157" s="17"/>
@@ -11392,7 +11392,7 @@
       <c r="J157" s="18"/>
       <c r="R157" s="19"/>
     </row>
-    <row r="158" spans="2:18" ht="14" customHeight="1">
+    <row r="158" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B158" s="16"/>
       <c r="C158" s="16"/>
       <c r="F158" s="17"/>
@@ -11402,7 +11402,7 @@
       <c r="J158" s="18"/>
       <c r="R158" s="19"/>
     </row>
-    <row r="159" spans="2:18" ht="14" customHeight="1">
+    <row r="159" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B159" s="16"/>
       <c r="C159" s="16"/>
       <c r="F159" s="17"/>
@@ -11412,7 +11412,7 @@
       <c r="J159" s="18"/>
       <c r="R159" s="19"/>
     </row>
-    <row r="160" spans="2:18" ht="14" customHeight="1">
+    <row r="160" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B160" s="16"/>
       <c r="C160" s="16"/>
       <c r="F160" s="17"/>
@@ -11422,7 +11422,7 @@
       <c r="J160" s="18"/>
       <c r="R160" s="19"/>
     </row>
-    <row r="161" spans="2:18" ht="14" customHeight="1">
+    <row r="161" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" s="16"/>
       <c r="C161" s="16"/>
       <c r="F161" s="17"/>
@@ -11432,7 +11432,7 @@
       <c r="J161" s="18"/>
       <c r="R161" s="19"/>
     </row>
-    <row r="162" spans="2:18" ht="14" customHeight="1">
+    <row r="162" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B162" s="16"/>
       <c r="C162" s="16"/>
       <c r="F162" s="17"/>
@@ -11442,7 +11442,7 @@
       <c r="J162" s="18"/>
       <c r="R162" s="19"/>
     </row>
-    <row r="163" spans="2:18" ht="14" customHeight="1">
+    <row r="163" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B163" s="16"/>
       <c r="C163" s="16"/>
       <c r="F163" s="17"/>
@@ -11452,7 +11452,7 @@
       <c r="J163" s="18"/>
       <c r="R163" s="19"/>
     </row>
-    <row r="164" spans="2:18" ht="14" customHeight="1">
+    <row r="164" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B164" s="16"/>
       <c r="C164" s="16"/>
       <c r="F164" s="17"/>
@@ -11462,7 +11462,7 @@
       <c r="J164" s="18"/>
       <c r="R164" s="19"/>
     </row>
-    <row r="165" spans="2:18" ht="14" customHeight="1">
+    <row r="165" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B165" s="16"/>
       <c r="C165" s="16"/>
       <c r="F165" s="17"/>
@@ -11472,7 +11472,7 @@
       <c r="J165" s="18"/>
       <c r="R165" s="19"/>
     </row>
-    <row r="166" spans="2:18" ht="14" customHeight="1">
+    <row r="166" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B166" s="16"/>
       <c r="C166" s="16"/>
       <c r="F166" s="17"/>
@@ -11482,7 +11482,7 @@
       <c r="J166" s="18"/>
       <c r="R166" s="19"/>
     </row>
-    <row r="167" spans="2:18" ht="14" customHeight="1">
+    <row r="167" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B167" s="16"/>
       <c r="C167" s="16"/>
       <c r="F167" s="17"/>
@@ -11492,7 +11492,7 @@
       <c r="J167" s="18"/>
       <c r="R167" s="19"/>
     </row>
-    <row r="168" spans="2:18" ht="14" customHeight="1">
+    <row r="168" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B168" s="16"/>
       <c r="C168" s="16"/>
       <c r="F168" s="17"/>
@@ -11502,7 +11502,7 @@
       <c r="J168" s="18"/>
       <c r="R168" s="19"/>
     </row>
-    <row r="169" spans="2:18" ht="14" customHeight="1">
+    <row r="169" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B169" s="16"/>
       <c r="C169" s="16"/>
       <c r="F169" s="17"/>
@@ -11512,7 +11512,7 @@
       <c r="J169" s="18"/>
       <c r="R169" s="19"/>
     </row>
-    <row r="170" spans="2:18" ht="14" customHeight="1">
+    <row r="170" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B170" s="16"/>
       <c r="C170" s="16"/>
       <c r="F170" s="17"/>
@@ -11522,7 +11522,7 @@
       <c r="J170" s="18"/>
       <c r="R170" s="19"/>
     </row>
-    <row r="171" spans="2:18" ht="14" customHeight="1">
+    <row r="171" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B171" s="16"/>
       <c r="C171" s="16"/>
       <c r="F171" s="17"/>
@@ -11532,7 +11532,7 @@
       <c r="J171" s="18"/>
       <c r="R171" s="19"/>
     </row>
-    <row r="172" spans="2:18" ht="14" customHeight="1">
+    <row r="172" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B172" s="16"/>
       <c r="C172" s="16"/>
       <c r="F172" s="17"/>
@@ -11542,7 +11542,7 @@
       <c r="J172" s="18"/>
       <c r="R172" s="19"/>
     </row>
-    <row r="173" spans="2:18" ht="14" customHeight="1">
+    <row r="173" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B173" s="16"/>
       <c r="C173" s="16"/>
       <c r="F173" s="17"/>
@@ -11552,7 +11552,7 @@
       <c r="J173" s="18"/>
       <c r="R173" s="19"/>
     </row>
-    <row r="174" spans="2:18" ht="14" customHeight="1">
+    <row r="174" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B174" s="16"/>
       <c r="C174" s="16"/>
       <c r="F174" s="17"/>
@@ -11562,7 +11562,7 @@
       <c r="J174" s="18"/>
       <c r="R174" s="19"/>
     </row>
-    <row r="175" spans="2:18" ht="14" customHeight="1">
+    <row r="175" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B175" s="16"/>
       <c r="C175" s="16"/>
       <c r="F175" s="17"/>
@@ -11572,7 +11572,7 @@
       <c r="J175" s="18"/>
       <c r="R175" s="19"/>
     </row>
-    <row r="176" spans="2:18" ht="14" customHeight="1">
+    <row r="176" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B176" s="16"/>
       <c r="C176" s="16"/>
       <c r="F176" s="17"/>
@@ -11582,7 +11582,7 @@
       <c r="J176" s="18"/>
       <c r="R176" s="19"/>
     </row>
-    <row r="177" spans="2:18" ht="14" customHeight="1">
+    <row r="177" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B177" s="16"/>
       <c r="C177" s="16"/>
       <c r="F177" s="17"/>
@@ -11592,7 +11592,7 @@
       <c r="J177" s="18"/>
       <c r="R177" s="19"/>
     </row>
-    <row r="178" spans="2:18" ht="14" customHeight="1">
+    <row r="178" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B178" s="16"/>
       <c r="C178" s="16"/>
       <c r="F178" s="17"/>
@@ -11602,7 +11602,7 @@
       <c r="J178" s="18"/>
       <c r="R178" s="19"/>
     </row>
-    <row r="179" spans="2:18" ht="14" customHeight="1">
+    <row r="179" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B179" s="16"/>
       <c r="C179" s="16"/>
       <c r="F179" s="17"/>
@@ -11612,7 +11612,7 @@
       <c r="J179" s="18"/>
       <c r="R179" s="19"/>
     </row>
-    <row r="180" spans="2:18" ht="14" customHeight="1">
+    <row r="180" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B180" s="16"/>
       <c r="C180" s="16"/>
       <c r="F180" s="17"/>
@@ -11622,7 +11622,7 @@
       <c r="J180" s="18"/>
       <c r="R180" s="19"/>
     </row>
-    <row r="181" spans="2:18" ht="14" customHeight="1">
+    <row r="181" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B181" s="16"/>
       <c r="C181" s="16"/>
       <c r="F181" s="17"/>
@@ -11632,7 +11632,7 @@
       <c r="J181" s="18"/>
       <c r="R181" s="19"/>
     </row>
-    <row r="182" spans="2:18" ht="14" customHeight="1">
+    <row r="182" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B182" s="16"/>
       <c r="C182" s="16"/>
       <c r="F182" s="17"/>
@@ -11642,7 +11642,7 @@
       <c r="J182" s="18"/>
       <c r="R182" s="19"/>
     </row>
-    <row r="183" spans="2:18" ht="14" customHeight="1">
+    <row r="183" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B183" s="16"/>
       <c r="C183" s="16"/>
       <c r="F183" s="17"/>
@@ -11652,7 +11652,7 @@
       <c r="J183" s="18"/>
       <c r="R183" s="19"/>
     </row>
-    <row r="184" spans="2:18" ht="14" customHeight="1">
+    <row r="184" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B184" s="16"/>
       <c r="C184" s="16"/>
       <c r="F184" s="17"/>
@@ -11662,7 +11662,7 @@
       <c r="J184" s="18"/>
       <c r="R184" s="19"/>
     </row>
-    <row r="185" spans="2:18" ht="14" customHeight="1">
+    <row r="185" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B185" s="16"/>
       <c r="C185" s="16"/>
       <c r="F185" s="17"/>
@@ -11672,7 +11672,7 @@
       <c r="J185" s="18"/>
       <c r="R185" s="19"/>
     </row>
-    <row r="186" spans="2:18" ht="14" customHeight="1">
+    <row r="186" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B186" s="16"/>
       <c r="C186" s="16"/>
       <c r="F186" s="17"/>
@@ -11682,7 +11682,7 @@
       <c r="J186" s="18"/>
       <c r="R186" s="19"/>
     </row>
-    <row r="187" spans="2:18" ht="14" customHeight="1">
+    <row r="187" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B187" s="16"/>
       <c r="C187" s="16"/>
       <c r="F187" s="17"/>
@@ -11692,7 +11692,7 @@
       <c r="J187" s="18"/>
       <c r="R187" s="19"/>
     </row>
-    <row r="188" spans="2:18" ht="14" customHeight="1">
+    <row r="188" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B188" s="16"/>
       <c r="C188" s="16"/>
       <c r="F188" s="17"/>
@@ -11702,7 +11702,7 @@
       <c r="J188" s="18"/>
       <c r="R188" s="19"/>
     </row>
-    <row r="189" spans="2:18" ht="14" customHeight="1">
+    <row r="189" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B189" s="16"/>
       <c r="C189" s="16"/>
       <c r="F189" s="17"/>
@@ -11712,7 +11712,7 @@
       <c r="J189" s="18"/>
       <c r="R189" s="19"/>
     </row>
-    <row r="190" spans="2:18" ht="14" customHeight="1">
+    <row r="190" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B190" s="16"/>
       <c r="C190" s="16"/>
       <c r="F190" s="17"/>
@@ -11722,7 +11722,7 @@
       <c r="J190" s="18"/>
       <c r="R190" s="19"/>
     </row>
-    <row r="191" spans="2:18" ht="14" customHeight="1">
+    <row r="191" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B191" s="16"/>
       <c r="C191" s="16"/>
       <c r="F191" s="17"/>
@@ -11732,7 +11732,7 @@
       <c r="J191" s="18"/>
       <c r="R191" s="19"/>
     </row>
-    <row r="192" spans="2:18" ht="14" customHeight="1">
+    <row r="192" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B192" s="16"/>
       <c r="C192" s="16"/>
       <c r="F192" s="17"/>
@@ -11742,7 +11742,7 @@
       <c r="J192" s="18"/>
       <c r="R192" s="19"/>
     </row>
-    <row r="193" spans="2:18" ht="14" customHeight="1">
+    <row r="193" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B193" s="16"/>
       <c r="C193" s="16"/>
       <c r="F193" s="17"/>
@@ -11752,7 +11752,7 @@
       <c r="J193" s="18"/>
       <c r="R193" s="19"/>
     </row>
-    <row r="194" spans="2:18" ht="14" customHeight="1">
+    <row r="194" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B194" s="16"/>
       <c r="C194" s="16"/>
       <c r="F194" s="17"/>
@@ -11762,7 +11762,7 @@
       <c r="J194" s="18"/>
       <c r="R194" s="19"/>
     </row>
-    <row r="195" spans="2:18" ht="14" customHeight="1">
+    <row r="195" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B195" s="16"/>
       <c r="C195" s="16"/>
       <c r="F195" s="17"/>
@@ -11772,7 +11772,7 @@
       <c r="J195" s="18"/>
       <c r="R195" s="19"/>
     </row>
-    <row r="196" spans="2:18" ht="14" customHeight="1">
+    <row r="196" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B196" s="16"/>
       <c r="C196" s="16"/>
       <c r="F196" s="17"/>
@@ -11782,7 +11782,7 @@
       <c r="J196" s="18"/>
       <c r="R196" s="19"/>
     </row>
-    <row r="197" spans="2:18" ht="14" customHeight="1">
+    <row r="197" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B197" s="16"/>
       <c r="C197" s="16"/>
       <c r="F197" s="17"/>
@@ -11792,7 +11792,7 @@
       <c r="J197" s="18"/>
       <c r="R197" s="19"/>
     </row>
-    <row r="198" spans="2:18" ht="14" customHeight="1">
+    <row r="198" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B198" s="16"/>
       <c r="C198" s="16"/>
       <c r="F198" s="17"/>
@@ -11802,7 +11802,7 @@
       <c r="J198" s="18"/>
       <c r="R198" s="19"/>
     </row>
-    <row r="199" spans="2:18" ht="14" customHeight="1">
+    <row r="199" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B199" s="16"/>
       <c r="C199" s="16"/>
       <c r="F199" s="17"/>
@@ -11812,7 +11812,7 @@
       <c r="J199" s="18"/>
       <c r="R199" s="19"/>
     </row>
-    <row r="200" spans="2:18" ht="14" customHeight="1">
+    <row r="200" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B200" s="16"/>
       <c r="C200" s="16"/>
       <c r="F200" s="17"/>
@@ -11822,7 +11822,7 @@
       <c r="J200" s="18"/>
       <c r="R200" s="19"/>
     </row>
-    <row r="201" spans="2:18" ht="14" customHeight="1">
+    <row r="201" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B201" s="16"/>
       <c r="C201" s="16"/>
       <c r="F201" s="17"/>
@@ -11832,7 +11832,7 @@
       <c r="J201" s="18"/>
       <c r="R201" s="19"/>
     </row>
-    <row r="202" spans="2:18" ht="14" customHeight="1">
+    <row r="202" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B202" s="16"/>
       <c r="C202" s="16"/>
       <c r="F202" s="17"/>
@@ -11842,7 +11842,7 @@
       <c r="J202" s="18"/>
       <c r="R202" s="19"/>
     </row>
-    <row r="203" spans="2:18" ht="14" customHeight="1">
+    <row r="203" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B203" s="16"/>
       <c r="C203" s="16"/>
       <c r="F203" s="17"/>
@@ -11852,7 +11852,7 @@
       <c r="J203" s="18"/>
       <c r="R203" s="19"/>
     </row>
-    <row r="204" spans="2:18" ht="14" customHeight="1">
+    <row r="204" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B204" s="16"/>
       <c r="C204" s="16"/>
       <c r="F204" s="17"/>
@@ -11862,7 +11862,7 @@
       <c r="J204" s="18"/>
       <c r="R204" s="19"/>
     </row>
-    <row r="205" spans="2:18" ht="14" customHeight="1">
+    <row r="205" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B205" s="16"/>
       <c r="C205" s="16"/>
       <c r="F205" s="17"/>
@@ -11872,7 +11872,7 @@
       <c r="J205" s="18"/>
       <c r="R205" s="19"/>
     </row>
-    <row r="206" spans="2:18" ht="14" customHeight="1">
+    <row r="206" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B206" s="16"/>
       <c r="C206" s="16"/>
       <c r="F206" s="17"/>
@@ -11882,7 +11882,7 @@
       <c r="J206" s="18"/>
       <c r="R206" s="19"/>
     </row>
-    <row r="207" spans="2:18" ht="14" customHeight="1">
+    <row r="207" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B207" s="16"/>
       <c r="C207" s="16"/>
       <c r="F207" s="17"/>
@@ -11892,7 +11892,7 @@
       <c r="J207" s="18"/>
       <c r="R207" s="19"/>
     </row>
-    <row r="208" spans="2:18" ht="14" customHeight="1">
+    <row r="208" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B208" s="16"/>
       <c r="C208" s="16"/>
       <c r="F208" s="17"/>
@@ -11902,7 +11902,7 @@
       <c r="J208" s="18"/>
       <c r="R208" s="19"/>
     </row>
-    <row r="209" spans="2:18" ht="14" customHeight="1">
+    <row r="209" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B209" s="16"/>
       <c r="C209" s="16"/>
       <c r="F209" s="17"/>
@@ -11912,7 +11912,7 @@
       <c r="J209" s="18"/>
       <c r="R209" s="19"/>
     </row>
-    <row r="210" spans="2:18" ht="14" customHeight="1">
+    <row r="210" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B210" s="16"/>
       <c r="C210" s="16"/>
       <c r="F210" s="17"/>
@@ -11922,7 +11922,7 @@
       <c r="J210" s="18"/>
       <c r="R210" s="19"/>
     </row>
-    <row r="211" spans="2:18" ht="14" customHeight="1">
+    <row r="211" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B211" s="16"/>
       <c r="C211" s="16"/>
       <c r="F211" s="17"/>
@@ -11932,7 +11932,7 @@
       <c r="J211" s="18"/>
       <c r="R211" s="19"/>
     </row>
-    <row r="212" spans="2:18" ht="14" customHeight="1">
+    <row r="212" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B212" s="16"/>
       <c r="C212" s="16"/>
       <c r="F212" s="17"/>
@@ -11942,7 +11942,7 @@
       <c r="J212" s="18"/>
       <c r="R212" s="19"/>
     </row>
-    <row r="213" spans="2:18" ht="14" customHeight="1">
+    <row r="213" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B213" s="16"/>
       <c r="C213" s="16"/>
       <c r="F213" s="17"/>
@@ -11952,7 +11952,7 @@
       <c r="J213" s="18"/>
       <c r="R213" s="19"/>
     </row>
-    <row r="214" spans="2:18" ht="14" customHeight="1">
+    <row r="214" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B214" s="16"/>
       <c r="C214" s="16"/>
       <c r="F214" s="17"/>
@@ -11962,7 +11962,7 @@
       <c r="J214" s="18"/>
       <c r="R214" s="19"/>
     </row>
-    <row r="215" spans="2:18" ht="14" customHeight="1">
+    <row r="215" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B215" s="16"/>
       <c r="C215" s="16"/>
       <c r="F215" s="17"/>
@@ -11972,7 +11972,7 @@
       <c r="J215" s="18"/>
       <c r="R215" s="19"/>
     </row>
-    <row r="216" spans="2:18" ht="14" customHeight="1">
+    <row r="216" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B216" s="16"/>
       <c r="C216" s="16"/>
       <c r="F216" s="17"/>
@@ -11982,7 +11982,7 @@
       <c r="J216" s="18"/>
       <c r="R216" s="19"/>
     </row>
-    <row r="217" spans="2:18" ht="14" customHeight="1">
+    <row r="217" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B217" s="16"/>
       <c r="C217" s="16"/>
       <c r="F217" s="17"/>
@@ -11992,7 +11992,7 @@
       <c r="J217" s="18"/>
       <c r="R217" s="19"/>
     </row>
-    <row r="218" spans="2:18" ht="14" customHeight="1">
+    <row r="218" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B218" s="16"/>
       <c r="C218" s="16"/>
       <c r="F218" s="17"/>
@@ -12002,7 +12002,7 @@
       <c r="J218" s="18"/>
       <c r="R218" s="19"/>
     </row>
-    <row r="219" spans="2:18" ht="14" customHeight="1">
+    <row r="219" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B219" s="16"/>
       <c r="C219" s="16"/>
       <c r="F219" s="17"/>
@@ -12012,7 +12012,7 @@
       <c r="J219" s="18"/>
       <c r="R219" s="19"/>
     </row>
-    <row r="220" spans="2:18" ht="14" customHeight="1">
+    <row r="220" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B220" s="16"/>
       <c r="C220" s="16"/>
       <c r="F220" s="17"/>
@@ -12022,7 +12022,7 @@
       <c r="J220" s="18"/>
       <c r="R220" s="19"/>
     </row>
-    <row r="221" spans="2:18" ht="14" customHeight="1">
+    <row r="221" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B221" s="16"/>
       <c r="C221" s="16"/>
       <c r="F221" s="17"/>
@@ -12032,7 +12032,7 @@
       <c r="J221" s="18"/>
       <c r="R221" s="19"/>
     </row>
-    <row r="222" spans="2:18" ht="14" customHeight="1">
+    <row r="222" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B222" s="16"/>
       <c r="C222" s="16"/>
       <c r="F222" s="17"/>
@@ -12042,7 +12042,7 @@
       <c r="J222" s="18"/>
       <c r="R222" s="19"/>
     </row>
-    <row r="223" spans="2:18" ht="14" customHeight="1">
+    <row r="223" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B223" s="16"/>
       <c r="C223" s="16"/>
       <c r="F223" s="17"/>
@@ -12052,7 +12052,7 @@
       <c r="J223" s="18"/>
       <c r="R223" s="19"/>
     </row>
-    <row r="224" spans="2:18" ht="14" customHeight="1">
+    <row r="224" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B224" s="16"/>
       <c r="C224" s="16"/>
       <c r="F224" s="17"/>
@@ -12062,7 +12062,7 @@
       <c r="J224" s="18"/>
       <c r="R224" s="19"/>
     </row>
-    <row r="225" spans="2:18" ht="14" customHeight="1">
+    <row r="225" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B225" s="16"/>
       <c r="C225" s="16"/>
       <c r="F225" s="17"/>
@@ -12072,7 +12072,7 @@
       <c r="J225" s="18"/>
       <c r="R225" s="19"/>
     </row>
-    <row r="226" spans="2:18" ht="14" customHeight="1">
+    <row r="226" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B226" s="16"/>
       <c r="C226" s="16"/>
       <c r="F226" s="17"/>
@@ -12082,7 +12082,7 @@
       <c r="J226" s="18"/>
       <c r="R226" s="19"/>
     </row>
-    <row r="227" spans="2:18" ht="14" customHeight="1">
+    <row r="227" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B227" s="16"/>
       <c r="C227" s="16"/>
       <c r="F227" s="17"/>
@@ -12092,7 +12092,7 @@
       <c r="J227" s="18"/>
       <c r="R227" s="19"/>
     </row>
-    <row r="228" spans="2:18" ht="14" customHeight="1">
+    <row r="228" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B228" s="16"/>
       <c r="C228" s="16"/>
       <c r="F228" s="17"/>
@@ -12102,7 +12102,7 @@
       <c r="J228" s="18"/>
       <c r="R228" s="19"/>
     </row>
-    <row r="229" spans="2:18" ht="14" customHeight="1">
+    <row r="229" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B229" s="16"/>
       <c r="C229" s="16"/>
       <c r="F229" s="17"/>
@@ -12112,7 +12112,7 @@
       <c r="J229" s="18"/>
       <c r="R229" s="19"/>
     </row>
-    <row r="230" spans="2:18" ht="14" customHeight="1">
+    <row r="230" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B230" s="16"/>
       <c r="C230" s="16"/>
       <c r="F230" s="17"/>
@@ -12122,7 +12122,7 @@
       <c r="J230" s="18"/>
       <c r="R230" s="19"/>
     </row>
-    <row r="231" spans="2:18" ht="14" customHeight="1">
+    <row r="231" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B231" s="16"/>
       <c r="C231" s="16"/>
       <c r="F231" s="17"/>
@@ -12132,7 +12132,7 @@
       <c r="J231" s="18"/>
       <c r="R231" s="19"/>
     </row>
-    <row r="232" spans="2:18" ht="14" customHeight="1">
+    <row r="232" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B232" s="16"/>
       <c r="C232" s="16"/>
       <c r="F232" s="17"/>
@@ -12142,7 +12142,7 @@
       <c r="J232" s="18"/>
       <c r="R232" s="19"/>
     </row>
-    <row r="233" spans="2:18" ht="14" customHeight="1">
+    <row r="233" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B233" s="16"/>
       <c r="C233" s="16"/>
       <c r="F233" s="17"/>
@@ -12152,7 +12152,7 @@
       <c r="J233" s="18"/>
       <c r="R233" s="19"/>
     </row>
-    <row r="234" spans="2:18" ht="14" customHeight="1">
+    <row r="234" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B234" s="16"/>
       <c r="C234" s="16"/>
       <c r="F234" s="17"/>
@@ -12162,7 +12162,7 @@
       <c r="J234" s="18"/>
       <c r="R234" s="19"/>
     </row>
-    <row r="235" spans="2:18" ht="14" customHeight="1">
+    <row r="235" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B235" s="16"/>
       <c r="C235" s="16"/>
       <c r="F235" s="17"/>
@@ -12172,7 +12172,7 @@
       <c r="J235" s="18"/>
       <c r="R235" s="19"/>
     </row>
-    <row r="236" spans="2:18" ht="14" customHeight="1">
+    <row r="236" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B236" s="16"/>
       <c r="C236" s="16"/>
       <c r="F236" s="17"/>
@@ -12182,7 +12182,7 @@
       <c r="J236" s="18"/>
       <c r="R236" s="19"/>
     </row>
-    <row r="237" spans="2:18" ht="14" customHeight="1">
+    <row r="237" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B237" s="16"/>
       <c r="C237" s="16"/>
       <c r="F237" s="17"/>
@@ -12192,7 +12192,7 @@
       <c r="J237" s="18"/>
       <c r="R237" s="19"/>
     </row>
-    <row r="238" spans="2:18" ht="14" customHeight="1">
+    <row r="238" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B238" s="16"/>
       <c r="C238" s="16"/>
       <c r="F238" s="17"/>
@@ -12202,7 +12202,7 @@
       <c r="J238" s="18"/>
       <c r="R238" s="19"/>
     </row>
-    <row r="239" spans="2:18" ht="14" customHeight="1">
+    <row r="239" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B239" s="16"/>
       <c r="C239" s="16"/>
       <c r="F239" s="17"/>
@@ -12212,7 +12212,7 @@
       <c r="J239" s="18"/>
       <c r="R239" s="19"/>
     </row>
-    <row r="240" spans="2:18" ht="14" customHeight="1">
+    <row r="240" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B240" s="16"/>
       <c r="C240" s="16"/>
       <c r="F240" s="17"/>
@@ -12222,7 +12222,7 @@
       <c r="J240" s="18"/>
       <c r="R240" s="19"/>
     </row>
-    <row r="241" spans="2:18" ht="14" customHeight="1">
+    <row r="241" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B241" s="16"/>
       <c r="C241" s="16"/>
       <c r="F241" s="17"/>
@@ -12232,7 +12232,7 @@
       <c r="J241" s="18"/>
       <c r="R241" s="19"/>
     </row>
-    <row r="242" spans="2:18" ht="14" customHeight="1">
+    <row r="242" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B242" s="16"/>
       <c r="C242" s="16"/>
       <c r="F242" s="17"/>
@@ -12242,7 +12242,7 @@
       <c r="J242" s="18"/>
       <c r="R242" s="19"/>
     </row>
-    <row r="243" spans="2:18" ht="14" customHeight="1">
+    <row r="243" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B243" s="16"/>
       <c r="C243" s="16"/>
       <c r="F243" s="17"/>
@@ -12252,7 +12252,7 @@
       <c r="J243" s="18"/>
       <c r="R243" s="19"/>
     </row>
-    <row r="244" spans="2:18" ht="14" customHeight="1">
+    <row r="244" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B244" s="16"/>
       <c r="C244" s="16"/>
       <c r="F244" s="17"/>
@@ -12262,7 +12262,7 @@
       <c r="J244" s="18"/>
       <c r="R244" s="19"/>
     </row>
-    <row r="245" spans="2:18" ht="14" customHeight="1">
+    <row r="245" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B245" s="16"/>
       <c r="C245" s="16"/>
       <c r="F245" s="17"/>
@@ -12272,7 +12272,7 @@
       <c r="J245" s="18"/>
       <c r="R245" s="19"/>
     </row>
-    <row r="246" spans="2:18" ht="14" customHeight="1">
+    <row r="246" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B246" s="16"/>
       <c r="C246" s="16"/>
       <c r="F246" s="17"/>
@@ -12282,7 +12282,7 @@
       <c r="J246" s="18"/>
       <c r="R246" s="19"/>
     </row>
-    <row r="247" spans="2:18" ht="14" customHeight="1">
+    <row r="247" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B247" s="16"/>
       <c r="C247" s="16"/>
       <c r="F247" s="17"/>
@@ -12292,7 +12292,7 @@
       <c r="J247" s="18"/>
       <c r="R247" s="19"/>
     </row>
-    <row r="248" spans="2:18" ht="14" customHeight="1">
+    <row r="248" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B248" s="16"/>
       <c r="C248" s="16"/>
       <c r="F248" s="17"/>
@@ -12302,7 +12302,7 @@
       <c r="J248" s="18"/>
       <c r="R248" s="19"/>
     </row>
-    <row r="249" spans="2:18" ht="14" customHeight="1">
+    <row r="249" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B249" s="16"/>
       <c r="C249" s="16"/>
       <c r="F249" s="17"/>
@@ -12312,7 +12312,7 @@
       <c r="J249" s="18"/>
       <c r="R249" s="19"/>
     </row>
-    <row r="250" spans="2:18" ht="14" customHeight="1">
+    <row r="250" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B250" s="16"/>
       <c r="C250" s="16"/>
       <c r="F250" s="17"/>
@@ -12322,7 +12322,7 @@
       <c r="J250" s="18"/>
       <c r="R250" s="19"/>
     </row>
-    <row r="251" spans="2:18" ht="14" customHeight="1">
+    <row r="251" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B251" s="16"/>
       <c r="C251" s="16"/>
       <c r="F251" s="17"/>
@@ -12332,7 +12332,7 @@
       <c r="J251" s="18"/>
       <c r="R251" s="19"/>
     </row>
-    <row r="252" spans="2:18" ht="14" customHeight="1">
+    <row r="252" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B252" s="16"/>
       <c r="C252" s="16"/>
       <c r="F252" s="17"/>
@@ -12342,7 +12342,7 @@
       <c r="J252" s="18"/>
       <c r="R252" s="19"/>
     </row>
-    <row r="253" spans="2:18" ht="14" customHeight="1">
+    <row r="253" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B253" s="16"/>
       <c r="C253" s="16"/>
       <c r="F253" s="17"/>
@@ -12352,7 +12352,7 @@
       <c r="J253" s="18"/>
       <c r="R253" s="19"/>
     </row>
-    <row r="254" spans="2:18" ht="14" customHeight="1">
+    <row r="254" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B254" s="16"/>
       <c r="C254" s="16"/>
       <c r="F254" s="17"/>
@@ -12362,7 +12362,7 @@
       <c r="J254" s="18"/>
       <c r="R254" s="19"/>
     </row>
-    <row r="255" spans="2:18" ht="14" customHeight="1">
+    <row r="255" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B255" s="16"/>
       <c r="C255" s="16"/>
       <c r="F255" s="17"/>
@@ -12372,7 +12372,7 @@
       <c r="J255" s="18"/>
       <c r="R255" s="19"/>
     </row>
-    <row r="256" spans="2:18" ht="14" customHeight="1">
+    <row r="256" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B256" s="16"/>
       <c r="C256" s="16"/>
       <c r="F256" s="17"/>
@@ -12382,7 +12382,7 @@
       <c r="J256" s="18"/>
       <c r="R256" s="19"/>
     </row>
-    <row r="257" spans="2:18" ht="14" customHeight="1">
+    <row r="257" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B257" s="16"/>
       <c r="C257" s="16"/>
       <c r="F257" s="17"/>
@@ -12392,7 +12392,7 @@
       <c r="J257" s="18"/>
       <c r="R257" s="19"/>
     </row>
-    <row r="258" spans="2:18" ht="14" customHeight="1">
+    <row r="258" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B258" s="16"/>
       <c r="C258" s="16"/>
       <c r="F258" s="17"/>
@@ -12402,7 +12402,7 @@
       <c r="J258" s="18"/>
       <c r="R258" s="19"/>
     </row>
-    <row r="259" spans="2:18" ht="14" customHeight="1">
+    <row r="259" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B259" s="16"/>
       <c r="C259" s="16"/>
       <c r="F259" s="17"/>
@@ -12412,7 +12412,7 @@
       <c r="J259" s="18"/>
       <c r="R259" s="19"/>
     </row>
-    <row r="260" spans="2:18" ht="14" customHeight="1">
+    <row r="260" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B260" s="16"/>
       <c r="C260" s="16"/>
       <c r="G260" s="18"/>
@@ -12420,7 +12420,7 @@
       <c r="I260" s="18"/>
       <c r="J260" s="18"/>
     </row>
-    <row r="261" spans="2:18" ht="14" customHeight="1">
+    <row r="261" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B261" s="16"/>
       <c r="C261" s="16"/>
       <c r="G261" s="18"/>
@@ -12428,7 +12428,7 @@
       <c r="I261" s="18"/>
       <c r="J261" s="18"/>
     </row>
-    <row r="262" spans="2:18" ht="14" customHeight="1">
+    <row r="262" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B262" s="16"/>
       <c r="C262" s="16"/>
       <c r="G262" s="18"/>
@@ -12436,7 +12436,7 @@
       <c r="I262" s="18"/>
       <c r="J262" s="18"/>
     </row>
-    <row r="263" spans="2:18" ht="14" customHeight="1">
+    <row r="263" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B263" s="16"/>
       <c r="C263" s="16"/>
       <c r="G263" s="18"/>
@@ -12444,7 +12444,7 @@
       <c r="I263" s="18"/>
       <c r="J263" s="18"/>
     </row>
-    <row r="264" spans="2:18" ht="14" customHeight="1">
+    <row r="264" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B264" s="16"/>
       <c r="C264" s="16"/>
       <c r="G264" s="18"/>
@@ -12452,7 +12452,7 @@
       <c r="I264" s="18"/>
       <c r="J264" s="18"/>
     </row>
-    <row r="265" spans="2:18" ht="14" customHeight="1">
+    <row r="265" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B265" s="16"/>
       <c r="C265" s="16"/>
       <c r="G265" s="18"/>
@@ -12460,7 +12460,7 @@
       <c r="I265" s="18"/>
       <c r="J265" s="18"/>
     </row>
-    <row r="266" spans="2:18" ht="14" customHeight="1">
+    <row r="266" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B266" s="16"/>
       <c r="C266" s="16"/>
       <c r="G266" s="18"/>
@@ -12468,7 +12468,7 @@
       <c r="I266" s="18"/>
       <c r="J266" s="18"/>
     </row>
-    <row r="267" spans="2:18" ht="14" customHeight="1">
+    <row r="267" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B267" s="16"/>
       <c r="C267" s="16"/>
       <c r="G267" s="18"/>
@@ -12476,7 +12476,7 @@
       <c r="I267" s="18"/>
       <c r="J267" s="18"/>
     </row>
-    <row r="268" spans="2:18" ht="14" customHeight="1">
+    <row r="268" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B268" s="16"/>
       <c r="C268" s="16"/>
       <c r="G268" s="18"/>
@@ -12484,7 +12484,7 @@
       <c r="I268" s="18"/>
       <c r="J268" s="18"/>
     </row>
-    <row r="269" spans="2:18" ht="14" customHeight="1">
+    <row r="269" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B269" s="16"/>
       <c r="C269" s="16"/>
       <c r="G269" s="18"/>
@@ -12492,7 +12492,7 @@
       <c r="I269" s="18"/>
       <c r="J269" s="18"/>
     </row>
-    <row r="270" spans="2:18" ht="14" customHeight="1">
+    <row r="270" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B270" s="16"/>
       <c r="C270" s="16"/>
       <c r="G270" s="18"/>
@@ -12500,7 +12500,7 @@
       <c r="I270" s="18"/>
       <c r="J270" s="18"/>
     </row>
-    <row r="271" spans="2:18" ht="14" customHeight="1">
+    <row r="271" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B271" s="16"/>
       <c r="C271" s="16"/>
       <c r="G271" s="18"/>
@@ -12508,7 +12508,7 @@
       <c r="I271" s="18"/>
       <c r="J271" s="18"/>
     </row>
-    <row r="272" spans="2:18" ht="14" customHeight="1">
+    <row r="272" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B272" s="16"/>
       <c r="C272" s="16"/>
       <c r="G272" s="18"/>
@@ -12516,7 +12516,7 @@
       <c r="I272" s="18"/>
       <c r="J272" s="18"/>
     </row>
-    <row r="273" spans="2:10" ht="14" customHeight="1">
+    <row r="273" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B273" s="16"/>
       <c r="C273" s="16"/>
       <c r="G273" s="18"/>
@@ -12524,7 +12524,7 @@
       <c r="I273" s="18"/>
       <c r="J273" s="18"/>
     </row>
-    <row r="274" spans="2:10" ht="14" customHeight="1">
+    <row r="274" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B274" s="16"/>
       <c r="C274" s="16"/>
       <c r="G274" s="18"/>
@@ -12532,7 +12532,7 @@
       <c r="I274" s="18"/>
       <c r="J274" s="18"/>
     </row>
-    <row r="275" spans="2:10" ht="14" customHeight="1">
+    <row r="275" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B275" s="16"/>
       <c r="C275" s="16"/>
       <c r="G275" s="18"/>
@@ -12540,7 +12540,7 @@
       <c r="I275" s="18"/>
       <c r="J275" s="18"/>
     </row>
-    <row r="276" spans="2:10" ht="14" customHeight="1">
+    <row r="276" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B276" s="16"/>
       <c r="C276" s="16"/>
       <c r="G276" s="18"/>
@@ -12548,7 +12548,7 @@
       <c r="I276" s="18"/>
       <c r="J276" s="18"/>
     </row>
-    <row r="277" spans="2:10" ht="14" customHeight="1">
+    <row r="277" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B277" s="16"/>
       <c r="C277" s="16"/>
       <c r="G277" s="18"/>
@@ -12556,7 +12556,7 @@
       <c r="I277" s="18"/>
       <c r="J277" s="18"/>
     </row>
-    <row r="278" spans="2:10" ht="14" customHeight="1">
+    <row r="278" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B278" s="16"/>
       <c r="C278" s="16"/>
       <c r="G278" s="18"/>
@@ -12564,7 +12564,7 @@
       <c r="I278" s="18"/>
       <c r="J278" s="18"/>
     </row>
-    <row r="279" spans="2:10" ht="14" customHeight="1">
+    <row r="279" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B279" s="16"/>
       <c r="C279" s="16"/>
       <c r="G279" s="18"/>
@@ -12572,7 +12572,7 @@
       <c r="I279" s="18"/>
       <c r="J279" s="18"/>
     </row>
-    <row r="280" spans="2:10" ht="14" customHeight="1">
+    <row r="280" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B280" s="16"/>
       <c r="C280" s="16"/>
       <c r="G280" s="18"/>
@@ -12580,7 +12580,7 @@
       <c r="I280" s="18"/>
       <c r="J280" s="18"/>
     </row>
-    <row r="281" spans="2:10" ht="14" customHeight="1">
+    <row r="281" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B281" s="16"/>
       <c r="C281" s="16"/>
       <c r="G281" s="18"/>
@@ -12588,7 +12588,7 @@
       <c r="I281" s="18"/>
       <c r="J281" s="18"/>
     </row>
-    <row r="282" spans="2:10" ht="14" customHeight="1">
+    <row r="282" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B282" s="16"/>
       <c r="C282" s="16"/>
       <c r="G282" s="18"/>
@@ -12596,7 +12596,7 @@
       <c r="I282" s="18"/>
       <c r="J282" s="18"/>
     </row>
-    <row r="283" spans="2:10" ht="14" customHeight="1">
+    <row r="283" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B283" s="16"/>
       <c r="C283" s="16"/>
       <c r="G283" s="18"/>
@@ -12604,7 +12604,7 @@
       <c r="I283" s="18"/>
       <c r="J283" s="18"/>
     </row>
-    <row r="284" spans="2:10" ht="14" customHeight="1">
+    <row r="284" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B284" s="16"/>
       <c r="C284" s="16"/>
       <c r="G284" s="18"/>
@@ -12612,7 +12612,7 @@
       <c r="I284" s="18"/>
       <c r="J284" s="18"/>
     </row>
-    <row r="285" spans="2:10" ht="14" customHeight="1">
+    <row r="285" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B285" s="16"/>
       <c r="C285" s="16"/>
       <c r="G285" s="18"/>
@@ -12620,7 +12620,7 @@
       <c r="I285" s="18"/>
       <c r="J285" s="18"/>
     </row>
-    <row r="286" spans="2:10" ht="14" customHeight="1">
+    <row r="286" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B286" s="16"/>
       <c r="C286" s="16"/>
       <c r="G286" s="18"/>
@@ -12628,7 +12628,7 @@
       <c r="I286" s="18"/>
       <c r="J286" s="18"/>
     </row>
-    <row r="287" spans="2:10" ht="14" customHeight="1">
+    <row r="287" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B287" s="16"/>
       <c r="C287" s="16"/>
       <c r="G287" s="18"/>
@@ -12636,7 +12636,7 @@
       <c r="I287" s="18"/>
       <c r="J287" s="18"/>
     </row>
-    <row r="288" spans="2:10" ht="14" customHeight="1">
+    <row r="288" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B288" s="16"/>
       <c r="C288" s="16"/>
       <c r="G288" s="18"/>
@@ -12644,7 +12644,7 @@
       <c r="I288" s="18"/>
       <c r="J288" s="18"/>
     </row>
-    <row r="289" spans="2:10" ht="14" customHeight="1">
+    <row r="289" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B289" s="16"/>
       <c r="C289" s="16"/>
       <c r="G289" s="18"/>
@@ -12652,7 +12652,7 @@
       <c r="I289" s="18"/>
       <c r="J289" s="18"/>
     </row>
-    <row r="290" spans="2:10" ht="14" customHeight="1">
+    <row r="290" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B290" s="16"/>
       <c r="C290" s="16"/>
       <c r="G290" s="18"/>
@@ -12660,7 +12660,7 @@
       <c r="I290" s="18"/>
       <c r="J290" s="18"/>
     </row>
-    <row r="291" spans="2:10" ht="14" customHeight="1">
+    <row r="291" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B291" s="16"/>
       <c r="C291" s="16"/>
       <c r="G291" s="18"/>
@@ -12668,7 +12668,7 @@
       <c r="I291" s="18"/>
       <c r="J291" s="18"/>
     </row>
-    <row r="292" spans="2:10" ht="14" customHeight="1">
+    <row r="292" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B292" s="16"/>
       <c r="C292" s="16"/>
       <c r="G292" s="18"/>
@@ -12676,7 +12676,7 @@
       <c r="I292" s="18"/>
       <c r="J292" s="18"/>
     </row>
-    <row r="293" spans="2:10" ht="14" customHeight="1">
+    <row r="293" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B293" s="16"/>
       <c r="C293" s="16"/>
       <c r="G293" s="18"/>
@@ -12684,7 +12684,7 @@
       <c r="I293" s="18"/>
       <c r="J293" s="18"/>
     </row>
-    <row r="294" spans="2:10" ht="14" customHeight="1">
+    <row r="294" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B294" s="16"/>
       <c r="C294" s="16"/>
       <c r="G294" s="18"/>
@@ -12692,7 +12692,7 @@
       <c r="I294" s="18"/>
       <c r="J294" s="18"/>
     </row>
-    <row r="295" spans="2:10" ht="14" customHeight="1">
+    <row r="295" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B295" s="16"/>
       <c r="C295" s="16"/>
       <c r="G295" s="18"/>
@@ -12700,7 +12700,7 @@
       <c r="I295" s="18"/>
       <c r="J295" s="18"/>
     </row>
-    <row r="296" spans="2:10" ht="14" customHeight="1">
+    <row r="296" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B296" s="16"/>
       <c r="C296" s="16"/>
       <c r="G296" s="18"/>
@@ -12708,7 +12708,7 @@
       <c r="I296" s="18"/>
       <c r="J296" s="18"/>
     </row>
-    <row r="297" spans="2:10" ht="14" customHeight="1">
+    <row r="297" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B297" s="16"/>
       <c r="C297" s="16"/>
       <c r="G297" s="18"/>
@@ -12716,7 +12716,7 @@
       <c r="I297" s="18"/>
       <c r="J297" s="18"/>
     </row>
-    <row r="298" spans="2:10" ht="14" customHeight="1">
+    <row r="298" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B298" s="16"/>
       <c r="C298" s="16"/>
       <c r="G298" s="18"/>
@@ -12724,7 +12724,7 @@
       <c r="I298" s="18"/>
       <c r="J298" s="18"/>
     </row>
-    <row r="299" spans="2:10" ht="14" customHeight="1">
+    <row r="299" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B299" s="16"/>
       <c r="C299" s="16"/>
       <c r="G299" s="18"/>
@@ -12732,7 +12732,7 @@
       <c r="I299" s="18"/>
       <c r="J299" s="18"/>
     </row>
-    <row r="300" spans="2:10" ht="14" customHeight="1">
+    <row r="300" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B300" s="16"/>
       <c r="C300" s="16"/>
       <c r="G300" s="18"/>
@@ -12740,7 +12740,7 @@
       <c r="I300" s="18"/>
       <c r="J300" s="18"/>
     </row>
-    <row r="301" spans="2:10" ht="14" customHeight="1">
+    <row r="301" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B301" s="16"/>
       <c r="C301" s="16"/>
       <c r="G301" s="18"/>
@@ -12748,7 +12748,7 @@
       <c r="I301" s="18"/>
       <c r="J301" s="18"/>
     </row>
-    <row r="302" spans="2:10" ht="14" customHeight="1">
+    <row r="302" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B302" s="16"/>
       <c r="C302" s="16"/>
       <c r="G302" s="18"/>
@@ -12756,7 +12756,7 @@
       <c r="I302" s="18"/>
       <c r="J302" s="18"/>
     </row>
-    <row r="303" spans="2:10" ht="14" customHeight="1">
+    <row r="303" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B303" s="16"/>
       <c r="C303" s="16"/>
       <c r="G303" s="18"/>
@@ -12764,7 +12764,7 @@
       <c r="I303" s="18"/>
       <c r="J303" s="18"/>
     </row>
-    <row r="304" spans="2:10" ht="14" customHeight="1">
+    <row r="304" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B304" s="16"/>
       <c r="C304" s="16"/>
       <c r="G304" s="18"/>
@@ -12772,7 +12772,7 @@
       <c r="I304" s="18"/>
       <c r="J304" s="18"/>
     </row>
-    <row r="305" spans="2:10" ht="14" customHeight="1">
+    <row r="305" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B305" s="16"/>
       <c r="C305" s="16"/>
       <c r="G305" s="18"/>
@@ -12780,7 +12780,7 @@
       <c r="I305" s="18"/>
       <c r="J305" s="18"/>
     </row>
-    <row r="306" spans="2:10" ht="14" customHeight="1">
+    <row r="306" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B306" s="16"/>
       <c r="C306" s="16"/>
       <c r="G306" s="18"/>
@@ -12788,7 +12788,7 @@
       <c r="I306" s="18"/>
       <c r="J306" s="18"/>
     </row>
-    <row r="307" spans="2:10" ht="14" customHeight="1">
+    <row r="307" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B307" s="16"/>
       <c r="C307" s="16"/>
       <c r="G307" s="18"/>
@@ -12796,7 +12796,7 @@
       <c r="I307" s="18"/>
       <c r="J307" s="18"/>
     </row>
-    <row r="308" spans="2:10" ht="14" customHeight="1">
+    <row r="308" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B308" s="16"/>
       <c r="C308" s="16"/>
       <c r="G308" s="18"/>
@@ -12804,124 +12804,124 @@
       <c r="I308" s="18"/>
       <c r="J308" s="18"/>
     </row>
-    <row r="309" spans="2:10" ht="14" customHeight="1">
+    <row r="309" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G309" s="18"/>
       <c r="H309" s="18"/>
       <c r="I309" s="18"/>
       <c r="J309" s="18"/>
     </row>
-    <row r="310" spans="2:10" ht="14" customHeight="1">
+    <row r="310" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G310" s="18"/>
       <c r="H310" s="18"/>
       <c r="I310" s="18"/>
       <c r="J310" s="18"/>
     </row>
-    <row r="311" spans="2:10" ht="14" customHeight="1">
+    <row r="311" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G311" s="18"/>
       <c r="H311" s="18"/>
       <c r="I311" s="18"/>
       <c r="J311" s="18"/>
     </row>
-    <row r="312" spans="2:10" ht="14" customHeight="1">
+    <row r="312" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G312" s="18"/>
       <c r="H312" s="18"/>
       <c r="I312" s="18"/>
       <c r="J312" s="18"/>
     </row>
-    <row r="313" spans="2:10" ht="14" customHeight="1">
+    <row r="313" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G313" s="18"/>
       <c r="H313" s="18"/>
       <c r="I313" s="18"/>
       <c r="J313" s="18"/>
     </row>
-    <row r="314" spans="2:10" ht="14" customHeight="1">
+    <row r="314" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G314" s="18"/>
       <c r="H314" s="18"/>
       <c r="I314" s="18"/>
       <c r="J314" s="18"/>
     </row>
-    <row r="315" spans="2:10" ht="14" customHeight="1">
+    <row r="315" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G315" s="18"/>
       <c r="H315" s="18"/>
       <c r="I315" s="18"/>
       <c r="J315" s="18"/>
     </row>
-    <row r="316" spans="2:10" ht="14" customHeight="1">
+    <row r="316" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G316" s="18"/>
       <c r="H316" s="18"/>
       <c r="I316" s="18"/>
       <c r="J316" s="18"/>
     </row>
-    <row r="317" spans="2:10" ht="14" customHeight="1">
+    <row r="317" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G317" s="18"/>
       <c r="H317" s="18"/>
       <c r="I317" s="18"/>
       <c r="J317" s="18"/>
     </row>
-    <row r="318" spans="2:10" ht="14" customHeight="1">
+    <row r="318" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G318" s="18"/>
       <c r="H318" s="18"/>
       <c r="I318" s="18"/>
       <c r="J318" s="18"/>
     </row>
-    <row r="319" spans="2:10" ht="14" customHeight="1">
+    <row r="319" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G319" s="18"/>
     </row>
-    <row r="320" spans="2:10" ht="14" customHeight="1">
+    <row r="320" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G320" s="18"/>
     </row>
-    <row r="321" spans="7:7" ht="14" customHeight="1">
+    <row r="321" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G321" s="18"/>
     </row>
-    <row r="322" spans="7:7" ht="14" customHeight="1">
+    <row r="322" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G322" s="18"/>
     </row>
-    <row r="323" spans="7:7" ht="14" customHeight="1">
+    <row r="323" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G323" s="18"/>
     </row>
-    <row r="324" spans="7:7" ht="14" customHeight="1">
+    <row r="324" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G324" s="18"/>
     </row>
-    <row r="325" spans="7:7" ht="14" customHeight="1">
+    <row r="325" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G325" s="18"/>
     </row>
-    <row r="326" spans="7:7" ht="14" customHeight="1">
+    <row r="326" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G326" s="18"/>
     </row>
-    <row r="327" spans="7:7" ht="14" customHeight="1">
+    <row r="327" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G327" s="18"/>
     </row>
-    <row r="328" spans="7:7" ht="14" customHeight="1">
+    <row r="328" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G328" s="18"/>
     </row>
-    <row r="329" spans="7:7" ht="14" customHeight="1">
+    <row r="329" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G329" s="18"/>
     </row>
-    <row r="330" spans="7:7" ht="14" customHeight="1">
+    <row r="330" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G330" s="18"/>
     </row>
-    <row r="331" spans="7:7" ht="14" customHeight="1">
+    <row r="331" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G331" s="18"/>
     </row>
-    <row r="332" spans="7:7" ht="14" customHeight="1">
+    <row r="332" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G332" s="18"/>
     </row>
-    <row r="333" spans="7:7" ht="14" customHeight="1">
+    <row r="333" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G333" s="18"/>
     </row>
-    <row r="334" spans="7:7" ht="14" customHeight="1">
+    <row r="334" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G334" s="18"/>
     </row>
-    <row r="335" spans="7:7" ht="14" customHeight="1">
+    <row r="335" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G335" s="18"/>
     </row>
-    <row r="336" spans="7:7" ht="14" customHeight="1">
+    <row r="336" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G336" s="18"/>
     </row>
-    <row r="337" spans="7:7" ht="14" customHeight="1">
+    <row r="337" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G337" s="18"/>
     </row>
-    <row r="338" spans="7:7" ht="14" customHeight="1">
+    <row r="338" spans="7:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G338" s="18"/>
     </row>
   </sheetData>
@@ -13796,12 +13796,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.5" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>379</v>
       </c>
@@ -13812,7 +13812,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>51</v>
       </c>
@@ -13823,7 +13823,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>52</v>
       </c>
@@ -13834,7 +13834,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>61</v>
       </c>
@@ -13845,7 +13845,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>60</v>
       </c>
@@ -13856,7 +13856,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>380</v>
       </c>
@@ -13867,7 +13867,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>56</v>
       </c>
@@ -13878,7 +13878,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>381</v>
       </c>
@@ -13889,7 +13889,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>59</v>
       </c>
@@ -13900,7 +13900,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>383</v>
       </c>
@@ -13911,7 +13911,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>54</v>
       </c>
@@ -13922,7 +13922,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
         <v>53</v>
       </c>
@@ -13933,7 +13933,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
         <v>57</v>
       </c>
@@ -13944,7 +13944,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
         <v>55</v>
       </c>
@@ -13955,7 +13955,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>62</v>
       </c>
@@ -13966,7 +13966,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
         <v>64</v>
       </c>
@@ -13977,7 +13977,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>63</v>
       </c>
@@ -13988,7 +13988,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
         <v>384</v>
       </c>
@@ -13999,7 +13999,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
         <v>386</v>
       </c>
@@ -14010,7 +14010,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
         <v>387</v>
       </c>
@@ -14021,7 +14021,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
         <v>389</v>
       </c>
@@ -14032,7 +14032,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
         <v>390</v>
       </c>
@@ -14043,7 +14043,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
         <v>67</v>
       </c>
@@ -14054,7 +14054,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="25" t="s">
         <v>68</v>
       </c>
@@ -14065,7 +14065,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
         <v>391</v>
       </c>
@@ -14076,7 +14076,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="25" t="s">
         <v>66</v>
       </c>
@@ -14087,7 +14087,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="25" t="s">
         <v>392</v>
       </c>
@@ -14098,7 +14098,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="25" t="s">
         <v>65</v>
       </c>
@@ -14109,7 +14109,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="25" t="s">
         <v>58</v>
       </c>
@@ -14120,7 +14120,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="25" t="s">
         <v>69</v>
       </c>
@@ -14145,57 +14145,57 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="69.83203125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>336</v>
       </c>
@@ -14213,17 +14213,17 @@
   </sheetPr>
   <dimension ref="A1:UW219"/>
   <sheetViews>
-    <sheetView topLeftCell="AW1" zoomScale="55" workbookViewId="0">
-      <selection activeCell="DQ14" sqref="DQ14"/>
+    <sheetView topLeftCell="FC2" zoomScale="85" workbookViewId="0">
+      <selection activeCell="GW9" sqref="GW9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="21" style="28" customWidth="1"/>
     <col min="5" max="569" width="2.5" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:564" s="31" customFormat="1" ht="25" customHeight="1">
+    <row r="1" spans="2:564" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="53" t="s">
         <v>393</v>
       </c>
@@ -15912,7 +15912,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="2" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1">
+    <row r="2" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="49" t="s">
         <v>450</v>
       </c>
@@ -16186,7 +16186,7 @@
       <c r="JG2" s="52"/>
       <c r="JH2" s="52"/>
     </row>
-    <row r="3" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1">
+    <row r="3" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="49" t="s">
         <v>454</v>
       </c>
@@ -16432,7 +16432,7 @@
       <c r="IO3" s="52"/>
       <c r="IP3" s="52"/>
     </row>
-    <row r="4" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1">
+    <row r="4" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="49" t="s">
         <v>457</v>
       </c>
@@ -16534,7 +16534,7 @@
       <c r="GO4" s="56"/>
       <c r="GP4" s="56"/>
     </row>
-    <row r="5" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1">
+    <row r="5" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="56"/>
       <c r="D5" s="56"/>
       <c r="E5" s="49"/>
@@ -16715,7 +16715,7 @@
       <c r="GX5" s="56"/>
       <c r="GY5" s="56"/>
     </row>
-    <row r="6" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1">
+    <row r="6" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="49" t="s">
         <v>471</v>
       </c>
@@ -16807,7 +16807,7 @@
       <c r="GB6" s="56"/>
       <c r="GC6" s="56"/>
     </row>
-    <row r="7" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1">
+    <row r="7" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="56"/>
       <c r="D7" s="56"/>
       <c r="E7" s="49"/>
@@ -16969,7 +16969,7 @@
       <c r="GK7" s="56"/>
       <c r="GL7" s="56"/>
     </row>
-    <row r="8" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1">
+    <row r="8" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="49" t="s">
         <v>476</v>
       </c>
@@ -17061,7 +17061,7 @@
       <c r="GH8" s="56"/>
       <c r="GI8" s="56"/>
     </row>
-    <row r="9" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1">
+    <row r="9" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="56"/>
       <c r="D9" s="56"/>
       <c r="E9" s="49"/>
@@ -17223,7 +17223,7 @@
       <c r="GQ9" s="56"/>
       <c r="GR9" s="56"/>
     </row>
-    <row r="10" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1">
+    <row r="10" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="49" t="s">
         <v>477</v>
       </c>
@@ -17361,7 +17361,7 @@
       <c r="HP10" s="56"/>
       <c r="HQ10" s="56"/>
     </row>
-    <row r="11" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1">
+    <row r="11" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="49" t="s">
         <v>481</v>
       </c>
@@ -17475,7 +17475,7 @@
       <c r="GX11" s="56"/>
       <c r="GY11" s="56"/>
     </row>
-    <row r="12" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1">
+    <row r="12" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="49" t="s">
         <v>482</v>
       </c>
@@ -17663,7 +17663,7 @@
       <c r="HV12" s="56"/>
       <c r="HW12" s="56"/>
     </row>
-    <row r="13" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1">
+    <row r="13" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="49" t="s">
         <v>484</v>
       </c>
@@ -17918,7 +17918,7 @@
       <c r="HY13" s="56"/>
       <c r="HZ13" s="56"/>
     </row>
-    <row r="14" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1">
+    <row r="14" spans="2:564" s="31" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="49" t="s">
         <v>489</v>
       </c>
@@ -18014,211 +18014,211 @@
       <c r="JN14" s="56"/>
       <c r="JO14" s="56"/>
     </row>
-    <row r="15" spans="2:564" ht="50" customHeight="1"/>
-    <row r="16" spans="2:564" ht="50" customHeight="1"/>
-    <row r="17" ht="50" customHeight="1"/>
-    <row r="18" ht="50" customHeight="1"/>
-    <row r="19" ht="50" customHeight="1"/>
-    <row r="20" ht="50" customHeight="1"/>
-    <row r="21" ht="50" customHeight="1"/>
-    <row r="22" ht="50" customHeight="1"/>
-    <row r="23" ht="50" customHeight="1"/>
-    <row r="24" ht="50" customHeight="1"/>
-    <row r="25" ht="50" customHeight="1"/>
-    <row r="26" ht="50" customHeight="1"/>
-    <row r="27" ht="50" customHeight="1"/>
-    <row r="28" ht="50" customHeight="1"/>
-    <row r="29" ht="50" customHeight="1"/>
-    <row r="30" ht="50" customHeight="1"/>
-    <row r="31" ht="50" customHeight="1"/>
-    <row r="32" ht="50" customHeight="1"/>
-    <row r="33" ht="50" customHeight="1"/>
-    <row r="34" ht="50" customHeight="1"/>
-    <row r="35" ht="50" customHeight="1"/>
-    <row r="36" ht="50" customHeight="1"/>
-    <row r="37" ht="50" customHeight="1"/>
-    <row r="38" ht="50" customHeight="1"/>
-    <row r="39" ht="50" customHeight="1"/>
-    <row r="40" ht="50" customHeight="1"/>
-    <row r="41" ht="50" customHeight="1"/>
-    <row r="42" ht="50" customHeight="1"/>
-    <row r="43" ht="50" customHeight="1"/>
-    <row r="44" ht="50" customHeight="1"/>
-    <row r="45" ht="50" customHeight="1"/>
-    <row r="46" ht="50" customHeight="1"/>
-    <row r="47" ht="50" customHeight="1"/>
-    <row r="48" ht="50" customHeight="1"/>
-    <row r="49" ht="50" customHeight="1"/>
-    <row r="50" ht="50" customHeight="1"/>
-    <row r="51" ht="50" customHeight="1"/>
-    <row r="52" ht="50" customHeight="1"/>
-    <row r="53" ht="50" customHeight="1"/>
-    <row r="54" ht="50" customHeight="1"/>
-    <row r="55" ht="50" customHeight="1"/>
-    <row r="56" ht="50" customHeight="1"/>
-    <row r="57" ht="50" customHeight="1"/>
-    <row r="58" ht="50" customHeight="1"/>
-    <row r="59" ht="50" customHeight="1"/>
-    <row r="60" ht="50" customHeight="1"/>
-    <row r="61" ht="50" customHeight="1"/>
-    <row r="62" ht="50" customHeight="1"/>
-    <row r="63" ht="50" customHeight="1"/>
-    <row r="64" ht="50" customHeight="1"/>
-    <row r="65" ht="50" customHeight="1"/>
-    <row r="66" ht="50" customHeight="1"/>
-    <row r="67" ht="50" customHeight="1"/>
-    <row r="68" ht="50" customHeight="1"/>
-    <row r="69" ht="50" customHeight="1"/>
-    <row r="70" ht="50" customHeight="1"/>
-    <row r="71" ht="50" customHeight="1"/>
-    <row r="72" ht="50" customHeight="1"/>
-    <row r="73" ht="50" customHeight="1"/>
-    <row r="74" ht="50" customHeight="1"/>
-    <row r="75" ht="50" customHeight="1"/>
-    <row r="76" ht="50" customHeight="1"/>
-    <row r="77" ht="50" customHeight="1"/>
-    <row r="78" ht="50" customHeight="1"/>
-    <row r="79" ht="50" customHeight="1"/>
-    <row r="80" ht="50" customHeight="1"/>
-    <row r="81" ht="50" customHeight="1"/>
-    <row r="82" ht="50" customHeight="1"/>
-    <row r="83" ht="50" customHeight="1"/>
-    <row r="84" ht="50" customHeight="1"/>
-    <row r="85" ht="50" customHeight="1"/>
-    <row r="86" ht="50" customHeight="1"/>
-    <row r="87" ht="50" customHeight="1"/>
-    <row r="88" ht="50" customHeight="1"/>
-    <row r="89" ht="50" customHeight="1"/>
-    <row r="90" ht="50" customHeight="1"/>
-    <row r="91" ht="50" customHeight="1"/>
-    <row r="92" ht="50" customHeight="1"/>
-    <row r="93" ht="50" customHeight="1"/>
-    <row r="94" ht="50" customHeight="1"/>
-    <row r="95" ht="50" customHeight="1"/>
-    <row r="96" ht="50" customHeight="1"/>
-    <row r="97" ht="50" customHeight="1"/>
-    <row r="98" ht="50" customHeight="1"/>
-    <row r="99" ht="50" customHeight="1"/>
-    <row r="100" ht="50" customHeight="1"/>
-    <row r="101" ht="50" customHeight="1"/>
-    <row r="102" ht="50" customHeight="1"/>
-    <row r="103" ht="50" customHeight="1"/>
-    <row r="104" ht="50" customHeight="1"/>
-    <row r="105" ht="50" customHeight="1"/>
-    <row r="106" ht="50" customHeight="1"/>
-    <row r="107" ht="50" customHeight="1"/>
-    <row r="108" ht="50" customHeight="1"/>
-    <row r="109" ht="50" customHeight="1"/>
-    <row r="110" ht="50" customHeight="1"/>
-    <row r="111" ht="50" customHeight="1"/>
-    <row r="112" ht="50" customHeight="1"/>
-    <row r="113" ht="50" customHeight="1"/>
-    <row r="114" ht="50" customHeight="1"/>
-    <row r="115" ht="50" customHeight="1"/>
-    <row r="116" ht="50" customHeight="1"/>
-    <row r="117" ht="50" customHeight="1"/>
-    <row r="118" ht="50" customHeight="1"/>
-    <row r="119" ht="50" customHeight="1"/>
-    <row r="120" ht="50" customHeight="1"/>
-    <row r="121" ht="50" customHeight="1"/>
-    <row r="122" ht="50" customHeight="1"/>
-    <row r="123" ht="50" customHeight="1"/>
-    <row r="124" ht="50" customHeight="1"/>
-    <row r="125" ht="50" customHeight="1"/>
-    <row r="126" ht="50" customHeight="1"/>
-    <row r="127" ht="50" customHeight="1"/>
-    <row r="128" ht="50" customHeight="1"/>
-    <row r="129" ht="50" customHeight="1"/>
-    <row r="130" ht="50" customHeight="1"/>
-    <row r="131" ht="50" customHeight="1"/>
-    <row r="132" ht="50" customHeight="1"/>
-    <row r="133" ht="50" customHeight="1"/>
-    <row r="134" ht="50" customHeight="1"/>
-    <row r="135" ht="50" customHeight="1"/>
-    <row r="136" ht="50" customHeight="1"/>
-    <row r="137" ht="50" customHeight="1"/>
-    <row r="138" ht="50" customHeight="1"/>
-    <row r="139" ht="50" customHeight="1"/>
-    <row r="140" ht="50" customHeight="1"/>
-    <row r="141" ht="50" customHeight="1"/>
-    <row r="142" ht="50" customHeight="1"/>
-    <row r="143" ht="50" customHeight="1"/>
-    <row r="144" ht="50" customHeight="1"/>
-    <row r="145" ht="50" customHeight="1"/>
-    <row r="146" ht="50" customHeight="1"/>
-    <row r="147" ht="50" customHeight="1"/>
-    <row r="148" ht="50" customHeight="1"/>
-    <row r="149" ht="50" customHeight="1"/>
-    <row r="150" ht="50" customHeight="1"/>
-    <row r="151" ht="50" customHeight="1"/>
-    <row r="152" ht="50" customHeight="1"/>
-    <row r="153" ht="50" customHeight="1"/>
-    <row r="154" ht="50" customHeight="1"/>
-    <row r="155" ht="50" customHeight="1"/>
-    <row r="156" ht="50" customHeight="1"/>
-    <row r="157" ht="50" customHeight="1"/>
-    <row r="158" ht="50" customHeight="1"/>
-    <row r="159" ht="50" customHeight="1"/>
-    <row r="160" ht="50" customHeight="1"/>
-    <row r="161" ht="50" customHeight="1"/>
-    <row r="162" ht="50" customHeight="1"/>
-    <row r="163" ht="50" customHeight="1"/>
-    <row r="164" ht="50" customHeight="1"/>
-    <row r="165" ht="50" customHeight="1"/>
-    <row r="166" ht="50" customHeight="1"/>
-    <row r="167" ht="50" customHeight="1"/>
-    <row r="168" ht="50" customHeight="1"/>
-    <row r="169" ht="50" customHeight="1"/>
-    <row r="170" ht="50" customHeight="1"/>
-    <row r="171" ht="50" customHeight="1"/>
-    <row r="172" ht="50" customHeight="1"/>
-    <row r="173" ht="50" customHeight="1"/>
-    <row r="174" ht="50" customHeight="1"/>
-    <row r="175" ht="50" customHeight="1"/>
-    <row r="176" ht="50" customHeight="1"/>
-    <row r="177" ht="50" customHeight="1"/>
-    <row r="178" ht="50" customHeight="1"/>
-    <row r="179" ht="50" customHeight="1"/>
-    <row r="180" ht="50" customHeight="1"/>
-    <row r="181" ht="50" customHeight="1"/>
-    <row r="182" ht="50" customHeight="1"/>
-    <row r="183" ht="50" customHeight="1"/>
-    <row r="184" ht="50" customHeight="1"/>
-    <row r="185" ht="50" customHeight="1"/>
-    <row r="186" ht="50" customHeight="1"/>
-    <row r="187" ht="50" customHeight="1"/>
-    <row r="188" ht="50" customHeight="1"/>
-    <row r="189" ht="50" customHeight="1"/>
-    <row r="190" ht="50" customHeight="1"/>
-    <row r="191" ht="50" customHeight="1"/>
-    <row r="192" ht="50" customHeight="1"/>
-    <row r="193" ht="50" customHeight="1"/>
-    <row r="194" ht="50" customHeight="1"/>
-    <row r="195" ht="50" customHeight="1"/>
-    <row r="196" ht="50" customHeight="1"/>
-    <row r="197" ht="50" customHeight="1"/>
-    <row r="198" ht="50" customHeight="1"/>
-    <row r="199" ht="50" customHeight="1"/>
-    <row r="200" ht="50" customHeight="1"/>
-    <row r="201" ht="50" customHeight="1"/>
-    <row r="202" ht="50" customHeight="1"/>
-    <row r="203" ht="50" customHeight="1"/>
-    <row r="204" ht="50" customHeight="1"/>
-    <row r="205" ht="50" customHeight="1"/>
-    <row r="206" ht="50" customHeight="1"/>
-    <row r="207" ht="50" customHeight="1"/>
-    <row r="208" ht="50" customHeight="1"/>
-    <row r="209" ht="50" customHeight="1"/>
-    <row r="210" ht="50" customHeight="1"/>
-    <row r="211" ht="50" customHeight="1"/>
-    <row r="212" ht="50" customHeight="1"/>
-    <row r="213" ht="50" customHeight="1"/>
-    <row r="214" ht="50" customHeight="1"/>
-    <row r="215" ht="50" customHeight="1"/>
-    <row r="216" ht="50" customHeight="1"/>
-    <row r="217" ht="50" customHeight="1"/>
-    <row r="218" ht="50" customHeight="1"/>
-    <row r="219" ht="50" customHeight="1"/>
+    <row r="15" spans="2:564" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="2:564" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="786">
     <mergeCell ref="CJ12:CU12"/>
@@ -19019,9 +19019,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>496</v>
       </c>
@@ -19042,12 +19042,12 @@
       <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="25" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="30" customHeight="1">
+    <row r="2" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="67" t="s">
         <v>497</v>
       </c>
@@ -19064,7 +19064,7 @@
       <c r="M2" s="56"/>
       <c r="N2" s="56"/>
     </row>
-    <row r="3" spans="2:14" ht="30" customHeight="1">
+    <row r="3" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="66">
         <v>45192</v>
       </c>
@@ -19081,7 +19081,7 @@
       <c r="M3" s="56"/>
       <c r="N3" s="56"/>
     </row>
-    <row r="4" spans="2:14" ht="28" customHeight="1">
+    <row r="4" spans="2:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="32" t="s">
         <v>498</v>
       </c>
@@ -19110,7 +19110,7 @@
       </c>
       <c r="N4" s="56"/>
     </row>
-    <row r="5" spans="2:14" ht="22" customHeight="1">
+    <row r="5" spans="2:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="33">
         <v>1</v>
       </c>
@@ -19137,7 +19137,7 @@
       </c>
       <c r="N5" s="56"/>
     </row>
-    <row r="6" spans="2:14" ht="22" customHeight="1">
+    <row r="6" spans="2:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="33">
         <v>2</v>
       </c>
@@ -19164,7 +19164,7 @@
       </c>
       <c r="N6" s="56"/>
     </row>
-    <row r="7" spans="2:14" ht="22" customHeight="1">
+    <row r="7" spans="2:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="33">
         <v>3</v>
       </c>
@@ -19191,7 +19191,7 @@
       </c>
       <c r="N7" s="56"/>
     </row>
-    <row r="8" spans="2:14" ht="22" customHeight="1">
+    <row r="8" spans="2:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="33">
         <v>4</v>
       </c>
@@ -19218,7 +19218,7 @@
       </c>
       <c r="N8" s="56"/>
     </row>
-    <row r="9" spans="2:14" ht="22" customHeight="1">
+    <row r="9" spans="2:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="33">
         <v>5</v>
       </c>

</xml_diff>